<commit_message>
Statistical Functions Finalized Commit
</commit_message>
<xml_diff>
--- a/Statistical Functions/Statistical Functions.xlsx
+++ b/Statistical Functions/Statistical Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Lambda-Development\Statistical Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1C9DD4-C313-4260-BD9E-49103696614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6081B28-FDAC-48BF-B0B2-26D38D165D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="1035" windowWidth="26370" windowHeight="14970" xr2:uid="{DB19F158-AACD-4F51-ACA6-D90EFF05B59D}"/>
   </bookViews>
@@ -16,21 +16,21 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="STAT_BENFORD_DIST">_xlfn.LAMBDA(_xlop.null, _xlfn.LET(_xlpm.list, _xlfn.TOCOL({1,2,3,4,5,6,7,8,9}), _xlpm.output, _xlfn.BYROW(_xlpm.list, _xlfn.LAMBDA(_xlpm.x, LOG(1 + (1 / MOD(_xlpm.x, 10))))), _xlpm.output))</definedName>
+    <definedName name="STAT_BENFORD_TABLE">_xlfn.LAMBDA(_xlop.mode, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "", UPPER(_xlpm.mode)), _xlpm.digits, _xlfn.SEQUENCE(9, , 1, 1), _xlpm.probs, _xlfn.BYROW(_xlpm.digits, _xlfn.LAMBDA(_xlpm.d,LOG10(1 + (1 / _xlpm.d)))), _xlpm.result, IF(_xlpm.mode = "LBL", _xlfn.HSTACK(_xlpm.digits, _xlpm.probs), _xlpm.probs), _xlpm.result))</definedName>
     <definedName name="STAT_FREQ_TABLE">_xlfn.LAMBDA(_xlpm.range,_xlop.mode, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "", UPPER(_xlpm.mode)), _xlpm.u_vals, _xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.range)), _xlpm.weights, _xlfn.BYROW(_xlpm.u_vals, _xlfn.LAMBDA(_xlpm.a, COUNTIF(_xlpm.range, _xlpm.a))), _xlpm.products, _xlpm.u_vals * _xlpm.weights, _xlpm.values_col, IF(_xlpm.mode = "LBL", _xlfn.VSTACK("Value", _xlpm.u_vals), _xlpm.u_vals), _xlpm.weights_col, IF(_xlpm.mode = "LBL", _xlfn.VSTACK("Weight", _xlpm.weights), _xlpm.weights), _xlpm.products_col, IF(_xlpm.mode = "LBL", _xlfn.VSTACK("Product", _xlpm.products), _xlpm.products), _xlfn.HSTACK(_xlpm.values_col, _xlpm.weights_col, _xlpm.products_col)))</definedName>
     <definedName name="STAT_GEO5">_xlfn.LAMBDA(_xlpm.range,_xlop.label,_xlop.prec, _xlfn.LET(_xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", UPPER(_xlpm.label)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.min_val, MIN(_xlpm.range), _xlpm.max_val, MAX(_xlpm.range), _xlpm.midrange, (_xlpm.min_val + _xlpm.max_val) / 2, _xlpm.lower_mid, (_xlpm.min_val + _xlpm.midrange) / 2, _xlpm.upper_mid, (_xlpm.midrange + _xlpm.max_val) / 2, _xlpm.raw_vals, _xlfn.VSTACK(_xlpm.min_val, _xlpm.lower_mid, _xlpm.midrange, _xlpm.upper_mid, _xlpm.max_val), _xlpm.rounded_vals, ROUND(_xlpm.raw_vals, _xlpm.prec), _xlpm.labels, _xlfn.VSTACK("Min", "Lower Mid", "Midrange", "Upper Mid", "Max"), _xlpm.output, IF(_xlpm.label = "LBL", _xlfn.HSTACK(_xlpm.labels, _xlpm.rounded_vals), _xlpm.rounded_vals), _xlpm.output))</definedName>
     <definedName name="STAT_MIDRANGE">_xlfn.LAMBDA(_xlpm.array,_xlop.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.count_val, COUNT(_xlpm.array), _xlpm.midrange, IF(_xlpm.count_val = 0, NA(), AVERAGE(MIN(_xlpm.array), MAX(_xlpm.array))), ROUND(_xlpm.midrange, _xlpm.prec)))</definedName>
     <definedName name="STAT_MINMAX">_xlfn.LAMBDA(_xlpm.array,_xlop.prec,_xlop.label,_xlop.layout, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", UPPER(_xlpm.label)), _xlpm.layout, IF(_xlfn.ISOMITTED(_xlpm.layout), "V", UPPER(_xlpm.layout)), _xlpm.min_val, ROUND(MIN(_xlpm.array), _xlpm.prec), _xlpm.max_val, ROUND(MAX(_xlpm.array), _xlpm.prec), _xlpm.result_lbl, _xlfn.VSTACK(_xlfn.HSTACK("Min", _xlpm.min_val), _xlfn.HSTACK("Max", _xlpm.max_val)), _xlpm.result_raw, IF(_xlpm.layout = "H", _xlfn.HSTACK(_xlpm.min_val, _xlpm.max_val), _xlfn.VSTACK(_xlpm.min_val, _xlpm.max_val)), IF(_xlpm.label = "LBL", _xlpm.result_lbl, _xlpm.result_raw)))</definedName>
+    <definedName name="STAT_PCT_OF_RANGE">_xlfn.LAMBDA(_xlpm.min,_xlpm.max,_xlpm.value,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.calc, (_xlpm.value - _xlpm.min) / (_xlpm.max - _xlpm.min), ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
+    <definedName name="STAT_PCT_REMAP">_xlfn.LAMBDA(_xlpm.StartMin,_xlpm.StartMax,_xlpm.Target,_xlpm.EndMin,_xlpm.EndMax,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.pct, (_xlpm.Target - _xlpm.StartMin) / (_xlpm.StartMax - _xlpm.StartMin), _xlpm.calc, _xlpm.pct * (_xlpm.EndMax - _xlpm.EndMin) + _xlpm.EndMin, ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
     <definedName name="STAT_QNTILES">_xlfn.LAMBDA(_xlpm.range,_xlop.divisions,_xlop.mode,_xlop.style,_xlop.precision, _xlfn.LET(_xlpm.divisions, IF(_xlfn.ISOMITTED(_xlpm.divisions), 10, _xlpm.divisions), _xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "", UPPER(_xlpm.mode)), _xlpm.style, IF(_xlfn.ISOMITTED(_xlpm.style), "ALL", UPPER(_xlpm.style)), _xlpm.precision, IF(_xlfn.ISOMITTED(_xlpm.precision), 3, _xlpm.precision), _xlpm.countVals, COUNT(_xlpm.range), _xlpm.isValid, ISNUMBER(_xlpm.divisions) * ISNUMBER(_xlpm.precision), IF(_xlpm.countVals = 0, SQRT("a"), IF(OR(NOT(_xlpm.isValid), _xlpm.divisions &lt; 1), SQRT(-1), _xlfn.LET(_xlpm.pctiles, _xlfn.SWITCH(_xlpm.style, "BIN", _xlfn.SEQUENCE(_xlpm.divisions - 1, 1, 1) / _xlpm.divisions, _xlfn.SEQUENCE(_xlpm.divisions + 1, 1, 0) / _xlpm.divisions), _xlpm.pct_labels, TEXT(_xlpm.pctiles, "0%"), _xlpm.pct_vals, ROUND(_xlfn.PERCENTILE.INC(_xlpm.range, _xlpm.pctiles), _xlpm.precision), IF(_xlpm.mode = "LBL", CHOOSE({1,2}, _xlpm.pct_labels, VALUE(_xlpm.pct_vals)), _xlfn.TOCOL(_xlpm.pct_vals)))))))</definedName>
-    <definedName name="STAT_RANGE_VALUE_OF_PERCENT">_xlfn.LAMBDA(_xlpm.min,_xlpm.max,_xlpm.pct,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.calc, _xlpm.pct * (_xlpm.max - _xlpm.min) + _xlpm.min, ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
-    <definedName name="STAT_RND_BENFORD">_xlfn.LAMBDA(_xlop.digits, _xlfn.LET(_xlpm.digits, IF(_xlfn.ISOMITTED(_xlpm.digits), 3, _xlpm.digits), _xlpm.numlist, _xlfn.SEQUENCE(9, 1, 1, 1), _xlpm.problist, {0.301,0.477,0.602,0.699,0.778,0.845,0.903,0.954,1}, _xlpm.random_numbers, _xlfn.RANDARRAY(_xlpm.digits, 1), _xlpm.generated_digits, INDEX(_xlpm.numlist, MATCH(_xlfn.XLOOKUP(_xlpm.random_numbers, _xlpm.problist, _xlpm.problist, , 1), _xlpm.problist, 1)), _xlpm.generated_number, _xlfn.TEXTJOIN("", TRUE, _xlpm.generated_digits), VALUE(_xlpm.generated_number)))</definedName>
-    <definedName name="STAT_RND_BENFORD_SINGLE">_xlfn.LAMBDA(_xlop.null, _xlfn.LET(_xlpm.numlist, _xlfn.SEQUENCE(9, , 1, 1), _xlpm.problist, {0.301,0.477,0.602,0.699,0.778,0.845,0.903,0.954,1}, _xlpm.prob, _xlfn.XLOOKUP(RAND(), _xlpm.problist, _xlpm.problist, , 1), _xlpm.prob_index, MATCH(_xlpm.prob, _xlpm.problist, 0), _xlpm.digit, INDEX(_xlpm.numlist, _xlpm.prob_index), VALUE(_xlpm.digit)))</definedName>
+    <definedName name="STAT_RND_BENFORD">_xlfn.LAMBDA(_xlop.digits, _xlfn.LET(_xlpm.digits, IF(_xlfn.ISOMITTED(_xlpm.digits), 1, _xlpm.digits), _xlpm.numlist, _xlfn.SEQUENCE(9, , 1, 1), _xlpm.problist, {0.301,0.477,0.602,0.699,0.778,0.845,0.903,0.954,1}, _xlpm.rand_nums, _xlfn.RANDARRAY(_xlpm.digits, 1), _xlpm.indices, MATCH(_xlfn.XLOOKUP(_xlpm.rand_nums, _xlpm.problist, _xlpm.problist, , 1), _xlpm.problist, 1), _xlpm.digits_generated, INDEX(_xlpm.numlist, _xlpm.indices), _xlpm.output, IF(_xlpm.digits = 1, VALUE(_xlpm.digits_generated), VALUE(_xlfn.TEXTJOIN("", TRUE, _xlpm.digits_generated))), _xlpm.output))</definedName>
     <definedName name="STAT_SELF_WTD_AVG">_xlfn.LAMBDA(_xlpm.range, _xlfn.LET(_xlpm.sum_vals, SUM(_xlpm.range), _xlpm.result, IF(_xlpm.sum_vals = 0, NA(), SUMPRODUCT(_xlpm.range, _xlpm.range) / _xlpm.sum_vals), _xlpm.result))</definedName>
     <definedName name="STAT_SHAPE">_xlfn.LAMBDA(_xlpm.range,_xlop.label,_xlop.prec, _xlfn.LET(_xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", UPPER(_xlpm.label)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.count_val, COUNT(_xlpm.range), _xlpm.μ, IF(_xlpm.count_val &gt; 0, AVERAGE(_xlpm.range), NA()), _xlpm.med, IF(_xlpm.count_val &gt; 0, MEDIAN(_xlpm.range), NA()), _xlpm.skew, IF(_xlpm.count_val &gt; 2, _xlfn.SKEW.P(_xlpm.range), NA()), _xlpm.kurt, IF(_xlpm.count_val &gt; 3, KURT(_xlpm.range), NA()), _xlpm.raw_vals, _xlfn.VSTACK(_xlpm.μ, _xlpm.med, _xlpm.skew, _xlpm.kurt), _xlpm.rounded_vals, ROUND(_xlpm.raw_vals, _xlpm.prec), _xlpm.labels, _xlfn.VSTACK("Mean (μ)", "Median", "Skew (P)", "Kurtosis (P)"), _xlpm.output, IF(_xlpm.label = "LBL", _xlfn.HSTACK(_xlpm.labels, _xlpm.rounded_vals), _xlpm.rounded_vals), _xlpm.output))</definedName>
-    <definedName name="STAT_STAT_RANGE_PERCENT_OF_VALUE">_xlfn.LAMBDA(_xlpm.min,_xlpm.max,_xlpm.value,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.calc, (_xlpm.value - _xlpm.min) / (_xlpm.max - _xlpm.min), ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
-    <definedName name="STAT_STAT_RANGE_PERCENT_TRANSFER">_xlfn.LAMBDA(_xlpm.StartMin,_xlpm.StartMax,_xlpm.Target,_xlpm.EndMin,_xlpm.EndMax,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.pct, (_xlpm.Target - _xlpm.StartMin) / (_xlpm.StartMax - _xlpm.StartMin), _xlpm.calc, _xlpm.pct * (_xlpm.EndMax - _xlpm.EndMin) + _xlpm.EndMin, ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
     <definedName name="STAT_STDERR">_xlfn.LAMBDA(_xlpm.array,_xlop.mode,_xlop.label,_xlop.precision, _xlfn.LET(_xlpm.precision, IF(_xlfn.ISOMITTED(_xlpm.precision), 3, _xlpm.precision), _xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", _xlpm.label), _xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "pop", LOWER(_xlpm.mode)), _xlpm.stderr, _xlfn.SWITCH(_xlpm.mode, "pop", _xlfn.STDEV.P(_xlpm.array) / SQRT(COUNTA(_xlpm.array)), "samp", _xlfn.STDEV.S(_xlpm.array) / SQRT(COUNTA(_xlpm.array)), _xlfn.STDEV.P(_xlpm.array) / SQRT(COUNTA(_xlpm.array))), _xlpm.result, ROUND(_xlpm.stderr, _xlpm.precision), IF(_xlpm.label = "lbl", "Standard Error: " &amp; _xlpm.result, _xlpm.result)))</definedName>
     <definedName name="STAT_SUMMARY">_xlfn.LAMBDA(_xlpm.range,_xlop.mode,_xlop.label,_xlop.prec, _xlfn.LET(_xlpm.raw_mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "SPAN", UPPER(_xlpm.mode)), _xlpm.mode, IF(OR(_xlpm.raw_mode = "SMRY", _xlpm.raw_mode = "SPAN"), _xlpm.raw_mode, 1 / 0), _xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", UPPER(_xlpm.label)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.μ, AVERAGE(_xlpm.range), _xlpm.σ, _xlfn.STDEV.P(_xlpm.range), _xlpm.min_val, MIN(_xlpm.range), _xlpm.max_val, MAX(_xlpm.range), _xlpm.med_val, MEDIAN(_xlpm.range), _xlpm.μ_minus_σ, _xlpm.μ - _xlpm.σ, _xlpm.μ_plus_σ, _xlpm.μ + _xlpm.σ, _xlpm.smry_vals, _xlfn.VSTACK(_xlpm.min_val, _xlpm.μ, _xlpm.med_val, _xlpm.max_val, _xlpm.σ), _xlpm.smry_labels, _xlfn.VSTACK("Min", "Mean (μ)", "Median", "Max", "Stdev (σ)"), _xlpm.span_vals, _xlfn.VSTACK(_xlpm.min_val, _xlpm.μ_minus_σ, _xlpm.μ, _xlpm.μ_plus_σ, _xlpm.max_val, _xlpm.σ), _xlpm.span_labels, _xlfn.VSTACK("Min", "μ − σ", "Mean (μ)", "μ + σ", "Max", "Stdev (σ)"), _xlpm.selected_vals, IF(_xlpm.mode = "SPAN", _xlpm.span_vals, _xlpm.smry_vals), _xlpm.selected_labels, IF(_xlpm.mode = "SPAN", _xlpm.span_labels, _xlpm.smry_labels), _xlpm.rounded_vals, ROUND(_xlpm.selected_vals, _xlpm.prec), _xlpm.result, IF(_xlpm.label = "LBL", _xlfn.HSTACK(_xlpm.selected_labels, _xlpm.rounded_vals), _xlpm.rounded_vals), _xlpm.result))</definedName>
+    <definedName name="STAT_VAL_BRACKET">_xlfn.LAMBDA(_xlpm.TestArray,_xlpm.Target,_xlop.incl,_xlop.mode,_xlop.lbl,_xlop.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.mode, UPPER(IF(_xlfn.ISOMITTED(_xlpm.mode), "VER", _xlpm.mode)), _xlpm.lbl, UPPER(IF(_xlfn.ISOMITTED(_xlpm.lbl), "", _xlpm.lbl)), _xlpm.lbl_val, _xlpm.lbl = "LBL", _xlpm.incl, UPPER(IF(_xlfn.ISOMITTED(_xlpm.incl), "INC", _xlpm.incl)), _xlpm.lower, MAX(_xlfn._xlws.FILTER(_xlpm.TestArray, _xlpm.TestArray &lt; _xlpm.Target)), _xlpm.upper, MIN(_xlfn._xlws.FILTER(_xlpm.TestArray, _xlpm.TestArray &gt; _xlpm.Target)), _xlpm.val_array, IF(_xlpm.incl = "INC", _xlfn.VSTACK(_xlpm.lower, _xlpm.Target, _xlpm.upper), _xlfn.VSTACK(_xlpm.lower, _xlpm.upper)), _xlpm.val_array_r, ROUND(_xlpm.val_array, _xlpm.prec), _xlpm.lbl_array, IF(_xlpm.incl = "INC", {"Lower";"Target";"Upper"}, {"Lower";"Upper"}), _xlpm.output, _xlfn.SWITCH(_xlpm.mode, "STR", "(" &amp; _xlfn.TEXTJOIN(" : ", , FIXED(_xlpm.val_array_r, _xlpm.prec)) &amp; ")", "HOR", IF(_xlpm.lbl_val, _xlfn.VSTACK(TRANSPOSE(_xlpm.lbl_array), TRANSPOSE(_xlpm.val_array_r)), TRANSPOSE(_xlpm.val_array_r)), "VER", IF(_xlpm.lbl_val, _xlfn.HSTACK(_xlpm.lbl_array, _xlpm.val_array_r), _xlpm.val_array_r), _xlpm.val_array_r), _xlpm.output))</definedName>
+    <definedName name="STAT_VALUE_OF_PCT">_xlfn.LAMBDA(_xlpm.min,_xlpm.max,_xlpm.pct,_xlop.decprec, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.decprec), 15, _xlpm.decprec), _xlpm.calc, _xlpm.pct * (_xlpm.max - _xlpm.min) + _xlpm.min, ROUND(_xlpm.calc, _xlpm.decprec)))</definedName>
     <definedName name="STAT_VOLUME">_xlfn.LAMBDA(_xlpm.range,_xlop.label,_xlop.prec, _xlfn.LET(_xlpm.label, IF(_xlfn.ISOMITTED(_xlpm.label), "", UPPER(_xlpm.label)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.count_val, COUNT(_xlpm.range), _xlpm.sum_val, SUM(_xlpm.range), _xlpm.mean_val, IF(_xlpm.count_val &gt; 0, AVERAGE(_xlpm.range), NA()), _xlpm.raw_vals, _xlfn.VSTACK(_xlpm.count_val, _xlpm.sum_val, _xlpm.mean_val), _xlpm.rounded_vals, ROUND(_xlpm.raw_vals, _xlpm.prec), _xlpm.labels, _xlfn.VSTACK("Count", "Sum", "Mean (μ)"), _xlpm.output, IF(_xlpm.label = "LBL", _xlfn.HSTACK(_xlpm.labels, _xlpm.rounded_vals), _xlpm.rounded_vals), _xlpm.output))</definedName>
     <definedName name="STAT_WTD_AVG">_xlfn.LAMBDA(_xlpm.wts,_xlpm.values, _xlfn.LET(_xlpm.len_match, COUNTA(_xlpm.wts) = COUNTA(_xlpm.values), _xlpm.total_wt, SUM(_xlpm.wts), _xlpm.result, IF(NOT(_xlpm.len_match) + (_xlpm.total_wt = 0), NA(), SUMPRODUCT(_xlpm.wts, _xlpm.values) / _xlpm.total_wt), _xlpm.result))</definedName>
   </definedNames>
@@ -443,7 +443,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="608" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="689" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -475,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB0C852-05ED-40A6-B28F-BD288E4DFB1C}">
-  <dimension ref="B3:M39"/>
+  <dimension ref="B3:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,13 +1065,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F45" t="str" cm="1">
+        <f t="array" ref="F45:G47">STAT_VAL_BRACKET(_xlfn.ANCHORARRAY(E3),6.2,,"VER", "LBL")</f>
+        <v>Lower</v>
+      </c>
+      <c r="G45">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F46" t="str">
+        <v>Target</v>
+      </c>
+      <c r="G46">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F47" t="str">
+        <v>Upper</v>
+      </c>
+      <c r="G47">
+        <v>6.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAXABuAFMAVABBAFQAXwBRAE4AVABJAEwARQBTAFwAbgBSAGUAdAB1AHIAbgBzACAAZQBxAHUAYQBsAGwAeQAgAHMAcABhAGMAZQBkACAAcQB1AGEAbgB0AGkAbABlAHMAIABmAHIAbwBtACAAYQAgAG4AdQBtAGUAcgBpAGMAIAByAGEAbgBnAGUALAAgAHcAaQB0AGgAIABvAHAAdABpAG8AbgBhAGwAIABsAGEAYgBlAGwAcwAgAGEAbgBkACAAYgBpAG4ALQBzAHQAeQBsAGUAIABzAGwAaQBjAGkAbgBnAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAIAAgACAAIAAgACAAFCAgAE4AdQBtAGUAcgBpAGMAIABpAG4AcAB1AHQAIAByAGEAbgBnAGUAIAAoAGUALgBnAC4ALAAgAEEAMQA6AEEAMQAwADAAKQBcAG4ALQAgAFsAZABpAHYAaQBzAGkAbwBuAHMAXQAgABQgIAAoAG8AcAB0AGkAbwBuAGEAbAApACAATgB1AG0AYgBlAHIAIABvAGYAIABxAHUAYQBuAHQAaQBsAGUAIABpAG4AdABlAHIAdgBhAGwAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAxADAAKQBcAG4ALQAgAFsAbQBvAGQAZQBdACAAIAAgACAAIAAgABQgIAAoAG8AcAB0AGkAbwBuAGEAbAApACAAVQBzAGUAIABcACIATABCAEwAXAAiACAAdABvACAAcgBlAHQAdQByAG4AIABsAGEAYgBlAGwAZQBkACAAMgAtAGMAbwBsAHUAbQBuACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAdgBhAGwAdQBlAHMAIABvAG4AbAB5ACkAXABuAC0AIABbAHMAdAB5AGwAZQBdACAAIAAgACAAIAAUICAAKABvAHAAdABpAG8AbgBhAGwAKQAgAFwAIgBBAEwATABcACIAIAAoAGQAZQBmAGEAdQBsAHQAKQAgAGkAbgBjAGwAdQBkAGUAcwAgADAAJQAgAGEAbgBkACAAMQAwADAAJQA7ACAAXAAiAEIASQBOAFwAIgAgAGUAeABjAGwAdQBkAGUAcwAgAGIAbwB0AGgAIABiAG8AdQBuAGQAYQByAGkAZQBzAFwAbgAtACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACAAFCAgACgAbwBwAHQAaQBvAG4AYQBsACkAIABEAGUAYwBpAG0AYQBsACAAcgBvAHUAbgBkAGkAbgBnACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIABxAHUAYQBuAHQAaQBsAGUAIAB2AGEAbAB1AGUAcwAsACAAbwByACAAYQAgADIALQBjAG8AbAB1AG0AbgAgAGwAYQBiAGUAbABlAGQAIABhAHIAcgBhAHkALAAgAGQAZQBwAGUAbgBkAGkAbgBnACAAbwBuACAAbQBvAGQAZQAuAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzADoAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAARABlAGMAaQBsAGUAcwBcAG4ALQAgAFMAVABBAFQAXwBRAE4AVABJAEwARQBTACgAQQAxADoAQQAxADAAMAAsACAANAAsACAAXAAiAEwAQgBMAFwAIgApACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAUQB1AGEAcgB0AGkAbABlAHMAIAB3AGkAdABoACAAbABhAGIAZQBsAHMAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAALAAgADEAMAAsACAALAAgAFwAIgBCAEkATgBcACIAKQAgACAAIAAgACAAIAAgACAAkiEgAEkAbgB0AGUAcgBuAGEAbAAgAGIAaQBuACAAYgBvAHUAbgBkAGEAcgBpAGUAcwAgACgAMQAwAC0AdABpAGwAZQBzACkAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAALAAgADIAMAAsACAAXAAiAEwAQgBMAFwAIgAsACAAXAAiAEIASQBOAFwAIgAsACAAMgApACAAkiEgAEwAYQBiAGUAbABlAGQAIABiAGkAbgAgAGMAdQB0AHMAIAB3AGkAdABoACAAMgAtAGQAaQBnAGkAdAAgAHIAbwB1AG4AZABpAG4AZwBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFEATgBUAEkATABFAFMAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAZABpAHYAaQBzAGkAbwBuAHMAXQAsACAAWwBtAG8AZABlAF0ALAAgAFsAcwB0AHkAbABlAF0ALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABOAG8AcgBtAGEAbABpAHoAZQAgAG8AcAB0AGkAbwBuAGEAbAAgAGEAcgBnAHUAbQBlAG4AdABzAFwAbgAgACAAIAAgACAAIAAgACAAZABpAHYAaQBzAGkAbwBuAHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAZABpAHYAaQBzAGkAbwBuAHMAKQAsACAAMQAwACwAIABkAGkAdgBpAHMAaQBvAG4AcwApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbQBvAGQAZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAHMAdAB5AGwAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABzAHQAeQBsAGUAKQAsACAAXAAiAEEATABMAFwAIgAsACAAVQBQAFAARQBSACgAcwB0AHkAbABlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwBpAHMAaQBvAG4AKQAsACAAMwAsACAAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFYAYQBsAGkAZABhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIABjAG8AdQBuAHQAVgBhAGwAcwAsACAAQwBPAFUATgBUACgAcgBhAG4AZwBlACkALABcAG4AIAAgACAAIAAgACAAIAAgAGkAcwBWAGEAbABpAGQALAAgAEkAUwBOAFUATQBCAEUAUgAoAGQAaQB2AGkAcwBpAG8AbgBzACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAGMAbwB1AG4AdABWAGEAbABzACAAPQAgADAALAAgAFMAUQBSAFQAKABcACIAYQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABPAFIAKABOAE8AVAAoAGkAcwBWAGEAbABpAGQAKQAsACAAZABpAHYAaQBzAGkAbwBuAHMAIAA8ACAAMQApACwAIABTAFEAUgBUACgALQAxACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFAAZQByAGMAZQBuAHQAaQBsAGUAIABjAHUAdAAgAHAAbwBpAG4AdABzACAAYgBhAHMAZQBkACAAbwBuACAAcwB0AHkAbABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcABjAHQAaQBsAGUAcwAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcwB0AHkAbABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBCAEkATgBcACIALAAgAFMARQBRAFUARQBOAEMARQAoAGQAaQB2AGkAcwBpAG8AbgBzACAALQAgADEALAAgADEALAAgADEAKQAgAC8AIABkAGkAdgBpAHMAaQBvAG4AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKABkAGkAdgBpAHMAaQBvAG4AcwAgACsAIAAxACwAIAAxACwAIAAwACkAIAAvACAAZABpAHYAaQBzAGkAbwBuAHMAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIAA9ACAAQQBMAEwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAATABhAGIAZQBsACAAZgBvAHIAbQBhAHQAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHAAYwB0AF8AbABhAGIAZQBsAHMALAAgAFQARQBYAFQAKABwAGMAdABpAGwAZQBzACwAIABcACIAMAAlAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQwBhAGwAYwB1AGwAYQB0AGUAIABxAHUAYQBuAHQAaQBsAGUAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHAAYwB0AF8AdgBhAGwAcwAsACAAUgBPAFUATgBEACgAUABFAFIAQwBFAE4AVABJAEwARQAuAEkATgBDACgAcgBhAG4AZwBlACwAIABwAGMAdABpAGwAZQBzACkALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AHQAaQBuAGcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBMAEIATABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAKAB7ADEALAAgADIAfQAsACAAcABjAHQAXwBsAGEAYgBlAGwAcwAsACAAVgBBAEwAVQBFACgAcABjAHQAXwB2AGEAbABzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAE8AQwBPAEwAKABwAGMAdABfAHYAYQBsAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBTAFQARABFAFIAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHMAdABhAG4AZABhAHIAZAAgAGUAcgByAG8AcgAgAG8AZgAgAHQAaABlACAAbQBlAGEAbgAgACgAUwBFAE0AKQAgAGYAbwByACAAYQAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIABhAHIAcgBhAHkAIAAgACAAIAAgAD0AIABUAGgAZQAgAGQAYQB0AGEAcwBlAHQAIAB0AG8AIABlAHYAYQBsAHUAYQB0AGUAXABuAC0AIABtAG8AZABlACAAIAAgACAAIAAgAD0AIABPAHAAdABpAG8AbgBhAGwAOwAgAFwAIgBwAG8AcABcACIAIABmAG8AcgAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAKQAsACAAXAAiAHMAYQBtAHAAXAAiACAAZgBvAHIAIABzAGEAbQBwAGwAZQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAEwAQgBMAFwAIgAgAHQAbwAgAHIAZQB0AHUAcgBuACAAYQAgAGwAYQBiAGUAbABlAGQAIABzAHQAcgBpAG4AZwAsACAAbwB0AGgAZQByAHcAaQBzAGUAIAByAGUAdAB1AHIAbgBzACAAbgB1AG0AZQByAGkAYwBcAG4ALQAgAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAG8AdQBuAGQAIAByAGUAcwB1AGwAdAAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4ATgBvAHQAZQBzADoAXABuAC0AIABTAHQAYQBuAGQAYQByAGQAIABlAHIAcgBvAHIAIAByAGUAZgBsAGUAYwB0AHMAIAB0AGgAZQAgAGUAeABwAGUAYwB0AGUAZAAgAHYAYQByAGkAYQBiAGkAbABpAHQAeQAgAG8AZgAgAHQAaABlACAAcwBhAG0AcABsAGUAIABtAGUAYQBuACwAIABhAHMAcwB1AG0AaQBuAGcAIAB0AGgAZQAgAGQAYQB0AGEAIAByAGUAcAByAGUAcwBlAG4AdABzACAAYQAgAHIAYQBuAGQAbwBtACAAcwBhAG0AcABsAGUALgBcAG4ALQAgAEkAZgAgAHQAaABlACAAZABhAHQAYQBzAGUAdAAgAHIAZQBwAHIAZQBzAGUAbgB0AHMAIAB0AGgAZQAgAGUAbgB0AGkAcgBlACAAcABvAHAAdQBsAGEAdABpAG8AbgAsACAAUwBFAE0AIABpAHMAIABtAGEAdABoAGUAbQBhAHQAaQBjAGEAbABsAHkAIAB2AGEAbABpAGQAIABiAHUAdAAgAG4AbwB0ACAAcAByAGEAYwB0AGkAYwBhAGwAbAB5ACAAbgBlAGMAZQBzAHMAYQByAHkAFCBpAHQAIABtAG8AZABlAGwAcwAgAGUAcgByAG8AcgAgAHQAaABhAHQAIABkAG8AZQBzAG4AGSB0ACAAZQB4AGkAcwB0AC4AXABuAFwAbgBFAHgAYQBtAHAAbABlADoAXABuAD0AUwBUAEEAVABfAFMAVABEAEUAUgBSACgAQQAxADoAQQAxADAAMAAsACAAXAAiAHMAYQBtAHAAXAAiACwAIABcACIATABCAEwAXAAiACwAIAAyACkAXABuAJIhIABcACIAUwB0AGEAbgBkAGEAcgBkACAARQByAHIAbwByADoAIAAxAC4AMgA3AFwAIgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFMAVABEAEUAUgBSACAAPQAgAEwAQQBNAEIARABBACgAYQByAHIAYQB5ACwAIABbAG0AbwBkAGUAXQAsACAAWwBsAGEAYgBlAGwAXQAsACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMAaQBzAGkAbwBuACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAaQBzAGkAbwBuACkALAAgADMALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAbABhAGIAZQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABcACIAcABvAHAAXAAiACwAIABMAE8AVwBFAFIAKABtAG8AZABlACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABzAHQAYQBuAGQAYQByAGQAIABlAHIAcgBvAHIAIABiAGEAcwBlAGQAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAAcwB0AGQAZQByAHIALAAgAFMAVwBJAFQAQwBIACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAHAAbwBwAFwAIgAsACAAUwBUAEQARQBWAC4AUAAoAGEAcgByAGEAeQApACAALwAgAFMAUQBSAFQAKABDAE8AVQBOAFQAQQAoAGEAcgByAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAHMAYQBtAHAAXAAiACwAIABTAFQARABFAFYALgBTACgAYQByAHIAYQB5ACkAIAAvACAAUwBRAFIAVAAoAEMATwBVAE4AVABBACgAYQByAHIAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAFQARABFAFYALgBQACgAYQByAHIAYQB5ACkAIAAvACAAUwBRAFIAVAAoAEMATwBVAE4AVABBACgAYQByAHIAYQB5ACkAKQAgACAALwAvACAAZgBhAGwAbABiAGEAYwBrAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABSAE8AVQBOAEQAKABzAHQAZABlAHIAcgAsACAAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIAbABiAGwAXAAiACwAIABcACIAUwB0AGEAbgBkAGEAcgBkACAARQByAHIAbwByADoAIABcACIAIAAmACAAcgBlAHMAdQBsAHQALAAgAHIAZQBzAHUAbAB0ACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8ATQBJAE4ATQBBAFgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABtAGkAbgBpAG0AdQBtACAAYQBuAGQAIABtAGEAeABpAG0AdQBtACAAbwBmACAAYQAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkALAAgAG8AcAB0AGkAbwBuAGEAbABsAHkAIABsAGEAYgBlAGwAZQBkACAAYQBzACAAYQAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AIABhAHIAcgBhAHkALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIABhAHIAcgBhAHkAIAAgAD0AIABUAGgAZQAgAGQAYQB0AGEAcwBlAHQAIAB0AG8AIABlAHYAYQBsAHUAYQB0AGUAXABuAC0AIABwAHIAZQBjACAAIAAgAD0AIABPAHAAdABpAG8AbgBhAGwAOwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAdABvACAAcgBvAHUAbgBkACAAcgBlAHMAdQBsAHQAIAAoAGQAZQBmAGEAdQBsAHQAOgAgADMAKQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAEwAQgBMAFwAIgAgAHIAZQB0AHUAcgBuAHMAIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAbwB1AHQAcAB1AHQAIAB3AGkAdABoACAAdABlAHgAdAAgAGEAbgBkACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQBzAFwAbgAtACAAbABhAHkAbwB1AHQAIAA9ACAATwBwAHQAaQBvAG4AYQBsADsAIABcACIASABcACIAIABmAG8AcgAgAGgAbwByAGkAegBvAG4AdABhAGwALAAgAFwAIgBWAFwAIgAgAGYAbwByACAAdgBlAHIAdABpAGMAYQBsACAAKABkAGUAZgBhAHUAbAB0ADoAIABcACIAVgBcACIAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAEQAZQBmAGEAdQBsAHQAOgAgAHsAbQBpAG4AOwAgAG0AYQB4AH0AIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AFwAbgAtACAASQBmACAAbABhAGIAZQBsACAAPQAgAFwAIgBMAEIATABcACIAOgAgAFwAbgAgACAAIAAgAE0AaQBuACAAIAAgACAAIAB8ACAAdgBhAGwAdQBlACAAIABcAG4AIAAgACAAIABNAGEAeAAgACAAIAAgACAAfAAgAHYAYQBsAHUAZQAgACAAXABuAC0AIABMAGEAeQBvAHUAdAAgAG0AbwBkAGUAIABhAGYAZgBlAGMAdABzACAAbwByAGkAZQBuAHQAYQB0AGkAbwBuACAAbwBuAGwAeQAgAGkAZgAgAGwAYQBiAGUAbAAgAGAiIABcACIATABCAEwAXAAiAFwAbgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAE0ASQBOAE0AQQBYACAAPQAgAEwAQQBNAEIARABBACgAYQByAHIAYQB5ACwAIABbAHAAcgBlAGMAXQAsACAAWwBsAGEAYgBlAGwAXQAsACAAWwBsAGEAeQBvAHUAdABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbABhAHkAbwB1AHQALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbABhAHkAbwB1AHQAKQAsACAAXAAiAFYAXAAiACwAIABVAFAAUABFAFIAKABsAGEAeQBvAHUAdAApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABSAE8AVQBOAEQAKABNAEkATgAoAGEAcgByAGEAeQApACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AYQB4AF8AdgBhAGwALAAgAFIATwBVAE4ARAAoAE0AQQBYACgAYQByAHIAYQB5ACkALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AF8AbABiAGwALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAbQBpAG4AXwB2AGEAbAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAE0AYQB4AFwAIgAsACAAbQBhAHgAXwB2AGEAbAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AF8AcgBhAHcALAAgAEkARgAoAGwAYQB5AG8AdQB0ACAAPQAgAFwAIgBIAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAG0AaQBuAF8AdgBhAGwALAAgAG0AYQB4AF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAG0AaQBuAF8AdgBhAGwALAAgAG0AYQB4AF8AdgBhAGwAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABJAEYAKABsAGEAYgBlAGwAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAAcgBlAHMAdQBsAHQAXwBsAGIAbAAsACAAcgBlAHMAdQBsAHQAXwByAGEAdwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBTAFUATQBNAEEAUgBZAFwAbgBcAG4AUAByAG8AdgBpAGQAZQBzACAAYQAgAGMAbwBuAGMAaQBzAGUAIABzAHQAYQB0AGkAcwB0AGkAYwBhAGwAIABzAHUAbQBtAGEAcgB5ACAAZgBvAHIAIABhACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHIAYQBuAGcAZQAgACAAPQAgAFQAaABlACAAZABhAHQAYQBzAGUAdAAgAHQAbwAgAGUAdgBhAGwAdQBhAHQAZQBcAG4ALQAgAG0AbwBkAGUAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAFMATQBSAFkAXAAiACAAbwByACAAXAAiAFMAUABBAE4AXAAiACAAKABkAGUAZgBhAHUAbAB0ADoAIABTAFAAQQBOACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIABTAE0AUgBZADoAIABNAGkAbgAsACAATQBlAGEAbgAsACAATQBlAGQAaQBhAG4ALAAgAE0AYQB4ACwAIABTAHQAZABlAHYAXABuACAAIAAgACAAIAAgACAAIAAgACAAIABTAFAAQQBOADoAIABNAGkAbgAsACAAvAMSIsMDLAAgAE0AZQBhAG4ALAAgALwDKwDDAywAIABNAGEAeAAsACAAUwB0AGQAZQB2AFwAbgAtACAAbABhAGIAZQBsACAAIAA9ACAATwBwAHQAaQBvAG4AYQBsADsAIABcACIATABCAEwAXAAiACAAcgBlAHQAdQByAG4AcwAgAGEAIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAbABhAGIAZQBsAGUAZAAgAGEAcgByAGEAeQBcAG4ALQAgAHAAcgBlAGMAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAAoAGQAZQBmAGEAdQBsAHQAOgAgADMAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAEEAIAB2AGUAcgB0AGkAYwBhAGwAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5ACAAbwByACAAbABhAGIAZQBsAGUAZAAgAG0AYQB0AHIAaQB4ACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlACAAYQBuAGQAIABsAGEAYgBlAGwAIABmAGwAYQBnAFwAbgBcAG4ATQBvAGQAZQAgAEQAZQBzAGMAcgBpAHAAdABpAG8AbgBzADoAXABuAC0AIABcACIAUwBNAFIAWQBcACIAOgAgAEIAYQBsAGEAbgBjAGUAZAAgAHMAbgBhAHAAcwBoAG8AdAAgAG8AZgAgAGMAZQBuAHQAZQByACAAYQBuAGQAIABzAHAAcgBlAGEAZABcAG4ALQAgAFwAIgBTAFAAQQBOAFwAIgA6ACAARQBtAHAAaABhAHMAaQB6AGUAcwAgAGQAaQBzAHQAcgBpAGIAdQB0AGkAbwBuACAAcwBoAGEAcABlACAAYQByAG8AdQBuAGQAIAB0AGgAZQAgAG0AZQBhAG4AIAAoALwDIACxACAAwwMpACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAdwBpAHQAaAAgAGMAbABlAGEAcgAgAGwAYQBiAGUAbABpAG4AZwAgAG8AZgAgAE0AZQBhAG4AIAAoALwDKQAgAGEAbgBkACAAUwB0AGQAZQB2ACAAKADDAykAIABvAG4AbAB5AFwAbgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFMAVQBNAE0AQQBSAFkAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbQBvAGQAZQBdACwAIABbAGwAYQBiAGUAbABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAByAGEAdwBfAG0AbwBkAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABcACIAUwBQAEEATgBcACIALAAgAFUAUABQAEUAUgAoAG0AbwBkAGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKAByAGEAdwBfAG0AbwBkAGUAIAA9ACAAXAAiAFMATQBSAFkAXAAiACwAIAByAGEAdwBfAG0AbwBkAGUAIAA9ACAAXAAiAFMAUABBAE4AXAAiACkALAAgAHIAYQB3AF8AbQBvAGQAZQAsACAAMQAvADAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgALwDLAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAwwMsACAAUwBUAEQARQBWAC4AUAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABNAEkATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAIABNAEEAWAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGUAZABfAHYAYQBsACwAIABNAEUARABJAEEATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIAC8A18AbQBpAG4AdQBzAF8AwwMsACAAvAMgAC0AIADDAywAXABuACAAIAAgACAAIAAgACAAIAC8A18AcABsAHUAcwBfAMMDLAAgALwDIAArACAAwwMsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFMAdQBtAG0AYQByAHkAIABtAG8AZABlADoAIABNAGkAbgAsACAATQBlAGEAbgAsACAATQBlAGQAaQBhAG4ALAAgAE0AYQB4ACwAIABTAHQAZABlAHYAXABuACAAIAAgACAAIAAgACAAIABzAG0AcgB5AF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBpAG4AXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8AywAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AZQBkAF8AdgBhAGwALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBhAHgAXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIADDA1wAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcwBtAHIAeQBfAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBNAGkAbgBcACIALAAgAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIATQBlAGQAaQBhAG4AXAAiACwAIABcACIATQBhAHgAXAAiACwAIABcACIAUwB0AGQAZQB2ACAAKADDAykAXAAiACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABTAHAAYQBuACAAbQBvAGQAZQA6ACAATQBpAG4ALAAgALwDEiLDAywAIABNAGUAYQBuACwAIAC8AysAwwMsACAATQBhAHgALAAgAMMDXABuACAAIAAgACAAIAAgACAAIABzAHAAYQBuAF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBpAG4AXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8A18AbQBpAG4AdQBzAF8AwwMsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8AywAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgALwDXwBwAGwAdQBzAF8AwwMsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAMMDXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABzAHAAYQBuAF8AbABhAGIAZQBsAHMALAAgAFYAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAXAAiALwDIAASIiAAwwNcACIALAAgAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIAvAMgACsAIADDA1wAIgAsACAAXAAiAE0AYQB4AFwAIgAsACAAXAAiAFMAdABkAGUAdgAgACgAwwMpAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcwBlAGwAZQBjAHQAZQBkAF8AdgBhAGwAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAUwBQAEEATgBcACIALAAgAHMAcABhAG4AXwB2AGEAbABzACwAIABzAG0AcgB5AF8AdgBhAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIABzAGUAbABlAGMAdABlAGQAXwBsAGEAYgBlAGwAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAUwBQAEEATgBcACIALAAgAHMAcABhAG4AXwBsAGEAYgBlAGwAcwAsACAAcwBtAHIAeQBfAGwAYQBiAGUAbABzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwAsACAAUgBPAFUATgBEACgAcwBlAGwAZQBjAHQAZQBkAF8AdgBhAGwAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAcwBlAGwAZQBjAHQAZQBkAF8AbABhAGIAZQBsAHMALAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAEcARQBPADUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGcAZQBvAG0AZQB0AHIAaQBjACAAZgBpAHYAZQAtAHAAbwBpAG4AdAAgAHMAdQBtAG0AYQByAHkAIABvAGYAIABhACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAuAFwAbgBcAG4AVABoAGkAcwAgAGkAcwAgAE4ATwBUACAAYQAgAHAAZQByAGMAZQBuAHQAaQBsAGUALQBiAGEAcwBlAGQAIABzAHUAbQBtAGEAcgB5ACAAKABsAGkAawBlACAAcQB1AGEAcgB0AGkAbABlAHMAKQAsAFwAbgBiAHUAdAAgAGEAIABzAHkAbQBtAGUAdAByAGkAYwAgAHAAbwBzAGkAdABpAG8AbgBhAGwAIABzAGMAYQBmAGYAbwBsAGQAIABhAGMAcgBvAHMAcwAgAHQAaABlACAATQBpAG4AEyBNAGEAeAAgAHMAcABhAG4ALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIAByAGEAbgBnAGUAIAAgACAAOgAgAFIAZQBxAHUAaQByAGUAZAAgAGEAcgByAGEAeQAgAG8AZgAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAcwBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIAB1AHMAZQAgAFwAIgBMAEIATABcACIAIABmAG8AcgAgAGwAYQBiAGUAbABlAGQAIAAyAC0AYwBvAGwAdQBtAG4AIABvAHUAdABwAHUAdAAgACgAZABlAGYAYQB1AGwAdAA6ACAAdQBuAGwAYQBiAGUAbABlAGQAKQBcAG4ALQAgAHAAcgBlAGMAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkAIABvAHIAIABsAGEAYgBlAGwAZQBkACAAbQBhAHQAcgBpAHgAIABpAG4AYwBsAHUAZABpAG4AZwA6AFwAbgAgACAAewBNAGkAbgAsACAATABvAHcAZQByACAATQBpAGQALAAgAE0AaQBkAHIAYQBuAGcAZQAsACAAVQBwAHAAZQByACAATQBpAGQALAAgAE0AYQB4AH0AXABuAFwAbgBGAG8AcgBtAHUAbABhAHMAOgBcAG4ALQAgAE0AaQBuACAAIAAgACAAIAAgACAAIAAgAD0AIABNAEkATgAoAHIAYQBuAGcAZQApAFwAbgAtACAATQBpAGQAcgBhAG4AZwBlACAAIAAgACAAPQAgACgATQBJAE4AIAArACAATQBBAFgAKQAgAC8AIAAyAFwAbgAtACAATABvAHcAZQByACAATQBpAGQAIAAgACAAPQAgACgATQBJAE4AIAArACAATQBpAGQAcgBhAG4AZwBlACkAIAAvACAAMgBcAG4ALQAgAFUAcABwAGUAcgAgAE0AaQBkACAAIAAgAD0AIAAoAE0AaQBkAHIAYQBuAGcAZQAgACsAIABNAEEAWAApACAALwAgADIAXABuAC0AIABNAGEAeAAgACAAIAAgACAAIAAgACAAIAA9ACAATQBBAFgAKAByAGEAbgBnAGUAKQBcAG4AXABuAE4AbwB0AGUAOgBcAG4ALQAgAFQAaABpAHMAIABmAHUAbgBjAHQAaQBvAG4AIABpAHMAIAAqACoAZABpAHMAdAByAGkAYgB1AHQAaQBvAG4ALQBhAGcAbgBvAHMAdABpAGMAKgAqAC4AIABJAHQAIAByAGUAcABvAHIAdABzACAAbgB1AG0AZQByAGkAYwAgAHAAbwBzAGkAdABpAG8AbgAgAG8AbgBsAHkALAAgAFwAbgAgACAAdwBpAHQAaABvAHUAdAAgAHIAZQBnAGEAcgBkACAAdABvACAAdABoAGUAIABmAHIAZQBxAHUAZQBuAGMAeQAgAG8AcgAgAGMAbAB1AHMAdABlAHIAaQBuAGcAIABvAGYAIAB2AGEAbAB1AGUAcwAuACAAVABoAGEAdAAgAG0AZQBhAG4AcwAgAGQAYQB0AGEAcwBlAHQAcwAgAFwAbgAgACAAdwBpAHQAaAAgAGgAaQBnAGgAbAB5ACAAcwBrAGUAdwBlAGQAIABvAHIAIAByAGUAcABlAHQAaQB0AGkAdgBlACAAdgBhAGwAdQBlAHMAIABtAGEAeQAgAHMAdABpAGwAbAAgAHkAaQBlAGwAZAAgAGUAdgBlAG4AbAB5ACAAcwBwAGEAYwBlAGQAIAByAGUAcwB1AGwAdABzACAAXABuACAAIABpAGYAIABNAGkAbgAgAGEAbgBkACAATQBhAHgAIAByAGUAbQBhAGkAbgAgAHQAaABlACAAcwBhAG0AZQAuACAASQB0ACAAaQBzACAAYgBlAHMAdAAgAHUAbgBkAGUAcgBzAHQAbwBvAGQAIABhAHMAIABhACAAKgBzAHkAbQBtAGUAdAByAHkAIABzAGMAYQBmAGYAbwBsAGQAKgAsACAAXABuACAAIABuAG8AdAAgAGEAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgBhAGwAIABhAG4AYQBsAHkAcwBpAHMALgBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBHAEUATwA1ACAAPQAgAEwAQQBNAEIARABBACgAcgBhAG4AZwBlACwAIABbAGwAYQBiAGUAbABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABsAGEAYgBlAGwALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbABhAGIAZQBsACkALAAgAFwAIgBcACIALAAgAFUAUABQAEUAUgAoAGwAYQBiAGUAbAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABNAEkATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAIABNAEEAWAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGkAZAByAGEAbgBnAGUALAAgACgAbQBpAG4AXwB2AGEAbAAgACsAIABtAGEAeABfAHYAYQBsACkAIAAvACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAbABvAHcAZQByAF8AbQBpAGQALAAgACgAbQBpAG4AXwB2AGEAbAAgACsAIABtAGkAZAByAGEAbgBnAGUAKQAgAC8AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAB1AHAAcABlAHIAXwBtAGkAZAAsACAAKABtAGkAZAByAGEAbgBnAGUAIAArACAAbQBhAHgAXwB2AGEAbAApACAALwAgADIALABcAG4AXABuACAAIAAgACAAIAAgACAAIAByAGEAdwBfAHYAYQBsAHMALAAgAFYAUwBUAEEAQwBLACgAbQBpAG4AXwB2AGEAbAAsACAAbABvAHcAZQByAF8AbQBpAGQALAAgAG0AaQBkAHIAYQBuAGcAZQAsACAAdQBwAHAAZQByAF8AbQBpAGQALAAgAG0AYQB4AF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMALAAgAFIATwBVAE4ARAAoAHIAYQB3AF8AdgBhAGwAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsAHMALAAgAFYAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAXAAiAEwAbwB3AGUAcgAgAE0AaQBkAFwAIgAsACAAXAAiAE0AaQBkAHIAYQBuAGcAZQBcACIALAAgAFwAIgBVAHAAcABlAHIAIABNAGkAZABcACIALAAgAFwAIgBNAGEAeABcACIAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0ACwAIABJAEYAKABsAGEAYgBlAGwAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAASABTAFQAQQBDAEsAKABsAGEAYgBlAGwAcwAsACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAKQAsACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBWAE8ATABVAE0ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABiAGEAcwBpAGMAIAB2AG8AbAB1AG0AZQB0AHIAaQBjACAAcwB0AGEAdABzACAAZgBvAHIAIABhACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHIAYQBuAGcAZQAgACAAIAA6ACAAUgBlAHEAdQBpAHIAZQBkACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIAB1AHMAZQAgAFwAIgBMAEIATABcACIAIABmAG8AcgAgAGwAYQBiAGUAbABlAGQAIAAyAC0AYwBvAGwAdQBtAG4AIABvAHUAdABwAHUAdABcAG4ALQAgAHAAcgBlAGMAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQwBvAHUAbgB0AFwAbgAtACAAUwB1AG0AXABuAC0AIABNAGUAYQBuACAAKAC8AykAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AVgBPAEwAVQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbABhAGIAZQBsAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGMAbwB1AG4AdABfAHYAYQBsACwAIABDAE8AVQBOAFQAKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcwB1AG0AXwB2AGEAbAAsACAAUwBVAE0AKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbQBlAGEAbgBfAHYAYQBsACwAIABJAEYAKABjAG8AdQBuAHQAXwB2AGEAbAAgAD4AIAAwACwAIABBAFYARQBSAEEARwBFACgAcgBhAG4AZwBlACkALAAgAE4AQQAoACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAYQB3AF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABjAG8AdQBuAHQAXwB2AGEAbAAsACAAcwB1AG0AXwB2AGEAbAAsACAAbQBlAGEAbgBfAHYAYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACwAIABSAE8AVQBOAEQAKAByAGEAdwBfAHYAYQBsAHMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBDAG8AdQBuAHQAXAAiACwAIABcACIAUwB1AG0AXAAiACwAIABcACIATQBlAGEAbgAgACgAvAMpAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAIABIAFMAVABBAEMASwAoAGwAYQBiAGUAbABzACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFMASABBAFAARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABjAGUAbgB0AHIAYQBsACAAdABlAG4AZABlAG4AYwB5ACAAYQBuAGQAIABzAGgAYQBwAGUAIABkAGUAcwBjAHIAaQBwAHQAbwByAHMAIABmAG8AcgAgAGEAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAIAAgADoAIABSAGUAcQB1AGkAcgBlAGQAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AFwAbgAtACAAbABhAGIAZQBsACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAOwAgAHUAcwBlACAAXAAiAEwAQgBMAFwAIgAgAGYAbwByACAAbABhAGIAZQBsAGUAZAAgADIALQBjAG8AbAB1AG0AbgAgAG8AdQB0AHAAdQB0AFwAbgAtACAAcAByAGUAYwAgACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAOwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAKABkAGUAZgBhAHUAbAB0ADoAIAAzACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABNAGUAYQBuACAAKAC8AykAXABuAC0AIABNAGUAZABpAGEAbgBcAG4ALQAgAFMAawBlAHcALgBQAFwAbgAtACAASwB1AHIAdAAuAFAAXABuAFwAbgBOAG8AdABlADoAXABuAC0AIABSAGUAdAB1AHIAbgBzACAAIwBOAC8AQQAgAGYAbwByACAAUwBrAGUAdwAgAG8AcgAgAEsAdQByAHQAbwBzAGkAcwAgAGkAZgAgAGYAZQB3AGUAcgAgAHQAaABhAG4AIAAzACAAdgBhAGwAdQBlAHMAIABhAHIAZQAgAHAAcgBlAHMAZQBuAHQALgBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBTAEgAQQBQAEUAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbABhAGIAZQBsAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGMAbwB1AG4AdABfAHYAYQBsACwAIABDAE8AVQBOAFQAKAByAGEAbgBnAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgALwDLAAgAEkARgAoAGMAbwB1AG4AdABfAHYAYQBsACAAPgAgADAALAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGUAZAAsACAASQBGACgAYwBvAHUAbgB0AF8AdgBhAGwAIAA+ACAAMAAsACAATQBFAEQASQBBAE4AKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuACAAIAAgACAAIAAgACAAIABzAGsAZQB3ACwAIABJAEYAKABjAG8AdQBuAHQAXwB2AGEAbAAgAD4AIAAyACwAIABTAEsARQBXAC4AUAAoAHIAYQBuAGcAZQApACwAIABOAEEAKAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGsAdQByAHQALAAgAEkARgAoAGMAbwB1AG4AdABfAHYAYQBsACAAPgAgADMALAAgAEsAVQBSAFQAKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcAXwB2AGEAbABzACwAIABWAFMAVABBAEMASwAoALwDLAAgAG0AZQBkACwAIABzAGsAZQB3ACwAIABrAHUAcgB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACwAIABSAE8AVQBOAEQAKAByAGEAdwBfAHYAYQBsAHMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIATQBlAGQAaQBhAG4AXAAiACwAIABcACIAUwBrAGUAdwAgACgAUAApAFwAIgAsACAAXAAiAEsAdQByAHQAbwBzAGkAcwAgACgAUAApAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAIABIAFMAVABBAEMASwAoAGwAYQBiAGUAbABzACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBTAFQAQQBUAF8ATABJAFMAVAAoAE8ATABEACkAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbQBvAGQAZQBdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAbQBvAGQAZQAgAD4AIAA2ACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsAF8AbABpAHMAdAAsACAAdAByAGEAbgBzAHAAbwBzAGUAKAB7AFwAIgBNAGkAbgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgDCA3sgXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAvANcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgDCA3ogXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBhAHgAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAwwNcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAGsAZQB3AC4AUABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBDAHQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUgBhAG4AZwBlAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE0AaQBkAHIAYQBuAGcAZQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAHUAbQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgCLHlwAIgB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgAHMAdABhAHQAcwAsACAAVABSAEEATgBTAFAATwBTAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEMASABPAE8AUwBFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAMQAsACAAMgAsACAAMwAsACAANAAsACAANQAsACAANgAsACAANwAsACAAOAAsACAAOQAsACAAMQAwACwAIAAxADEALAAgADEAMgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAE0ASQBOACgAcgBhAG4AZwBlACkALAAgAHAAcgBlAGMAKQAsACAALwAvACAAbQBpAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAgAC0AIABTAFQARABFAFYALgBQACgAcgBhAG4AZwBlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABwAHIAZQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIAAvAC8AIAAtAHMAaQBnAG0AYQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAFgARQBEACgAQQBWAEUAUgBBAEcARQAoAHIAYQBuAGcAZQApACwAIABwAHIAZQBjACkALAAgAC8ALwAgAG0AZQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAgACsAIABTAFQARABFAFYALgBQACgAcgBhAG4AZwBlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABwAHIAZQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIAAvAC8AIAArAHMAaQBnAG0AYQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAFgARQBEACgATQBBAFgAKAByAGEAbgBnAGUAKQAsACAAcAByAGUAYwApACwAIAAvAC8AIABtAGEAeABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAFgARQBEACgAUwBUAEQARQBWAC4AUAAoAHIAYQBuAGcAZQApACwAIABwAHIAZQBjACkALAAgAC8ALwAgAHMAaQBnAG0AYQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAFgARQBEACgAUwBLAEUAVwAuAFAAKAByAGEAbgBnAGUAKQAsACAAcAByAGUAYwApACwAIAAvAC8AIABzAGsAZQB3AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkAWABFAEQAKABDAE8AVQBOAFQAKAByAGEAbgBnAGUAKQAsACAAMAApACwAIAAvAC8AIABjAG8AdQBuAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAE0AQQBYACgAcgBhAG4AZwBlACkAIAAtACAATQBJAE4AKAByAGEAbgBnAGUAKQAsACAAcAByAGUAYwApACwAIAAvAC8AIAByAGEAbgBnAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAEEAVgBFAFIAQQBHAEUAKABNAEkATgAoAHIAYQBuAGcAZQApACwATQBBAFgAKAByAGEAbgBnAGUAKQApACwAcAByAGUAYwApACwAIAAvAC8AIABtAGkAZAByAGEAbgBnAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAFMAVQBNACgAcgBhAG4AZwBlACkALAAgAHAAcgBlAGMAKQAsACAALwAvACAAcwB1AG0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAG0AZQBkAGkAYQBuACgAcgBhAG4AZwBlACkALAAgAHAAcgBlAGMAKQAsACAALwAvACAAbQBlAGQAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAAQwBIAE8ATwBTAEUAKAB7ADEALAAgADIAfQAsACAAbABhAGIAZQBsAF8AbABpAHMAdAAsACAAVgBBAEwAVQBFACgAcwB0AGEAdABzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4ALAAgAHMAdwBpAHQAYwBoACgAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIABvAHUAdABwAHUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIABjAGgAbwBvAHMAZQByAG8AdwBzACgAbwB1AHQAcAB1AHQALAAgADEALAAgADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIABDAGgAbwBvAHMAZQByAG8AdwBzACgAbwB1AHQAcAB1AHQALAAgADEALAAgADMALAAgADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzACwAIABDAGgAbwBvAHMAZQByAG8AdwBzACgAbwB1AHQAcAB1AHQALAAgADEALAAgADIALAAgADMALAAgADQALAAgADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA0ACwAIABDAGgAbwBvAHMAZQByAG8AdwBzACgAbwB1AHQAcAB1AHQALAAgADEALAAgADIALAAgADMALAAgADQALAAgADUALAAgADEAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUALAAgAEMAaABvAG8AcwBlAHIAbwB3AHMAKABvAHUAdABwAHUAdAAsACAAMQAsACAAMgAsACAAMwAsACAANAAsACAANQAsACAANgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADYALAAgAEMAaABvAG8AcwBlAHIAbwB3AHMAKABvAHUAdABwAHUAdAAsACAAMQAsACAAMgAsACAAMwAsACAANAAsACAANQAsACAANgAsACAAMQAxACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAFwAbgAgACAAIAAgACkAXABuAFwAbgApADsAXABuAFwAbgAvACoAIABTAFQAQQBUAF8ATQBJAEQAUgBBAE4ARwBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbQBpAGQAcgBhAG4AZwBlACAAbwBmACAAYQAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkAOgAgAHQAaABlACAAYQB2AGUAcgBhAGcAZQAgAG8AZgAgAGkAdABzACAATQBpAG4AIABhAG4AZAAgAE0AYQB4AC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAYQByAHIAYQB5ACAAOgAgAHIAZQBxAHUAaQByAGUAZAAgAG4AdQBtAGUAcgBpAGMAIAByAGEAbgBnAGUAXABuAC0AIABwAHIAZQBjACAAIAA6ACAAbwBwAHQAaQBvAG4AYQBsACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHMAaQBuAGcAbABlACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQA6ACAAKABNAEkATgAgACsAIABNAEEAWAApACAALwAgADIAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8ATQBJAEQAUgBBAE4ARwBFACAAPQAgAEwAQQBNAEIARABBACgAYQByAHIAYQB5ACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAAMwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABjAG8AdQBuAHQAXwB2AGEAbAAsACAAQwBPAFUATgBUACgAYQByAHIAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AaQBkAHIAYQBuAGcAZQAsACAASQBGACgAYwBvAHUAbgB0AF8AdgBhAGwAIAA9ACAAMAAsACAATgBBACgAKQAsACAAQQBWAEUAUgBBAEcARQAoAE0ASQBOACgAYQByAHIAYQB5ACkALAAgAE0AQQBYACgAYQByAHIAYQB5ACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABtAGkAZAByAGEAbgBnAGUALAAgAHAAcgBlAGMAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAEYAUgBFAFEAXwBUAEEAQgBMAEUAXABuAFwAbgBHAGUAbgBlAHIAYQB0AGUAcwAgAGEAIABmAHIAZQBxAHUAZQBuAGMAeQAgAHQAYQBiAGwAZQAgAGYAcgBvAG0AIABhACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHIAYQBuAGcAZQAgADoAIAByAGUAcQB1AGkAcgBlAGQAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0AFwAbgAtACAAbQBvAGQAZQAgACAAOgAgAG8AcAB0AGkAbwBuAGEAbAAgAGsAZQB5AHcAbwByAGQAIAAoAFwAIgBMAEIATABcACIAIAB0AG8AIABpAG4AYwBsAHUAZABlACAAYwBvAGwAdQBtAG4AIABoAGUAYQBkAGUAcgBzADsAIABkAGUAZgBhAHUAbAB0ACAAPQAgAG4AbwAgAGgAZQBhAGQAZQByAHMAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAEEAIAAzAC0AYwBvAGwAdQBtAG4AIABzAHAAaQBsAGwAZQBkACAAYQByAHIAYQB5ADoAXABuACAAIAAgACAAIiAgAEMAbwBsAHUAbQBuACAAMQA6ACAAVQBuAGkAcQB1AGUAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAiICAAQwBvAGwAdQBtAG4AIAAyADoAIABGAHIAZQBxAHUAZQBuAGMAeQAgACgAYwBvAHUAbgB0ACkAXABuACAAIAAgACAAIiAgAEMAbwBsAHUAbQBuACAAMwA6ACAAVwBlAGkAZwBoAHQAZQBkACAAcAByAG8AZAB1AGMAdAAgACgAdgBhAGwAdQBlACAA1wAgAGMAbwB1AG4AdAApAFwAbgBcAG4ATgBvAHQAZQBzADoAXABuAC0AIABTAG8AcgB0AGUAZAAgAGkAbgAgAGEAcwBjAGUAbgBkAGkAbgBnACAAbwByAGQAZQByAFwAbgAtACAASQBuAGMAbAB1AGQAZQBzACAAaABlAGEAZABlAHIAcwAgAGkAZgAgAG0AbwBkAGUAIAA9ACAAXAAiAEwAQgBMAFwAIgBcAG4ALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABtAG8AZABlACAAYQBuAGEAbAB5AHMAaQBzACwAIAB3AGUAaQBnAGgAdABlAGQAIABtAGUAYQBuAHMALAAgAGEAbgBkACAAZABpAHMAdAByAGkAYgB1AHQAaQBvAG4AIABvAHYAZQByAHYAaQBlAHcAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8ARgBSAEUAUQBfAFQAQQBCAEwARQAgAD0AIABMAEEATQBCAEQAQQAoAHIAYQBuAGcAZQAsACAAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAASABhAG4AZABsAGUAIABsAGEAYgBlAGwAIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABtAG8AZABlACkALAAgAFwAIgBcACIALAAgAFUAUABQAEUAUgAoAG0AbwBkAGUAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAUAByAGUAcABhAHIAZQAgAHUAbgBpAHEAdQBlACAAdgBhAGwAdQBlAHMAIABpAG4AIABzAG8AcgB0AGUAZAAgAG8AcgBkAGUAcgBcAG4AIAAgACAAIAAgACAAIAAgAHUAXwB2AGEAbABzACwAIABTAE8AUgBUACgAVQBOAEkAUQBVAEUAKAByAGEAbgBnAGUAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARgByAGUAcQB1AGUAbgBjAHkAIABjAG8AdQBuAHQAcwAgAHAAZQByACAAdQBuAGkAcQB1AGUAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAIAAgACAAIAB3AGUAaQBnAGgAdABzACwAIABCAFkAUgBPAFcAKAB1AF8AdgBhAGwAcwAsACAATABBAE0AQgBEAEEAKABhACwAIABDAE8AVQBOAFQASQBGACgAcgBhAG4AZwBlACwAIABhACkAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAVwBlAGkAZwBoAHQAZQBkACAAdgBhAGwAdQBlACAA1wAgAGYAcgBlAHEAdQBlAG4AYwB5AFwAbgAgACAAIAAgACAAIAAgACAAcAByAG8AZAB1AGMAdABzACwAIAB1AF8AdgBhAGwAcwAgACoAIAB3AGUAaQBnAGgAdABzACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAQQBkAGQAIABjAG8AbAB1AG0AbgAgAGgAZQBhAGQAZQByAHMAIABpAGYAIABcACIATABCAEwAXAAiACAAbQBvAGQAZQBcAG4AIAAgACAAIAAgACAAIAAgAHYAYQBsAHUAZQBzAF8AYwBvAGwALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAAVgBTAFQAQQBDAEsAKABcACIAVgBhAGwAdQBlAFwAIgAsACAAdQBfAHYAYQBsAHMAKQAsACAAdQBfAHYAYQBsAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAdwBlAGkAZwBoAHQAcwBfAGMAbwBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBMAEIATABcACIALAAgAFYAUwBUAEEAQwBLACgAXAAiAFcAZQBpAGcAaAB0AFwAIgAsACAAdwBlAGkAZwBoAHQAcwApACwAIAB3AGUAaQBnAGgAdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBvAGQAdQBjAHQAcwBfAGMAbwBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBMAEIATABcACIALAAgAFYAUwBUAEEAQwBLACgAXAAiAFAAcgBvAGQAdQBjAHQAXAAiACwAIABwAHIAbwBkAHUAYwB0AHMAKQAsACAAcAByAG8AZAB1AGMAdABzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABGAGkAbgBhAGwAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAdgBhAGwAdQBlAHMAXwBjAG8AbAAsACAAdwBlAGkAZwBoAHQAcwBfAGMAbwBsACwAIABwAHIAbwBkAHUAYwB0AHMAXwBjAG8AbAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8AVwBUAEQAXwBBAFYARwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHcAZQBpAGcAaAB0AGUAZAAgAGEAdgBlAHIAYQBnAGUAIABvAGYAIABhACAAdgBhAGwAdQBlACAAcwBlAHQAIABiAGEAcwBlAGQAIABvAG4AIABhACAAbQBhAHQAYwBoAGkAbgBnACAAdwBlAGkAZwBoAHQAIABzAGUAdAAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHcAdABzACAAIAAgACAAOgAgAGEAcgByAGEAeQAgAG8AZgAgAHcAZQBpAGcAaAB0AHMAXABuAC0AIAB2AGEAbAB1AGUAcwAgADoAIABhAHIAcgBhAHkAIABvAGYAIAB2AGEAbAB1AGUAcwAgACgAcwBhAG0AZQAgAGwAZQBuAGcAdABoACAAYQBzACAAdwBlAGkAZwBoAHQAcwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAVwBlAGkAZwBoAHQAZQBkACAAYQB2AGUAcgBhAGcAZQAgAD0AIABTAFUATQBQAFIATwBEAFUAQwBUACgAdwB0AHMALAAgAHYAYQBsAHUAZQBzACkAIAAvACAAUwBVAE0AKAB3AHQAcwApAFwAbgAtACAAUgBlAHQAdQByAG4AcwAgACMATgAvAEEAIABpAGYAIABpAG4AcAB1AHQAIABsAGUAbgBnAHQAaABzACAAbQBpAHMAbQBhAHQAYwBoACAAbwByACAAdwBlAGkAZwBoAHQAIABzAHUAbQAgAGkAcwAgAHoAZQByAG8AXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AVwBUAEQAXwBBAFYARwAgAD0AIABMAEEATQBCAEQAQQAoAHcAdABzACwAIAB2AGEAbAB1AGUAcwAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABsAGUAbgBfAG0AYQB0AGMAaAAsACAAQwBPAFUATgBUAEEAKAB3AHQAcwApACAAPQAgAEMATwBVAE4AVABBACgAdgBhAGwAdQBlAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAdABvAHQAYQBsAF8AdwB0ACwAIABTAFUATQAoAHcAdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABsAGUAbgBfAG0AYQB0AGMAaAApACAAKwAgACgAdABvAHQAYQBsAF8AdwB0ACAAPQAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAEEAKAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMAVQBNAFAAUgBPAEQAVQBDAFQAKAB3AHQAcwAsACAAdgBhAGwAdQBlAHMAKQAgAC8AIAB0AG8AdABhAGwAXwB3AHQAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABTAFQAQQBUAF8AUwBFAEwARgBfAFcAVABEAF8AQQBWAEcAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAHMAZQBsAGYALQB3AGUAaQBnAGgAdABlAGQAIABhAHYAZQByAGEAZwBlACAAbwBmACAAdgBhAGwAdQBlAHMALAAgAHcAaABlAHIAZQAgAGUAYQBjAGgAIAB2AGEAbAB1AGUAIABpAHMAIAB0AHIAZQBhAHQAZQBkACAAYQBzACAAaQB0AHMAIABvAHcAbgAgAHcAZQBpAGcAaAB0AC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAOgAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIACjAygAeABiHbIAKQAgAC8AIACjAygAeABiHSkAXABuAC0AIABSAGUAdAB1AHIAbgBzACAAIwBOAC8AQQAgAGkAZgAgAHQAbwB0AGEAbAAgAHMAdQBtACAAPQAgADAAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AUwBFAEwARgBfAFcAVABEAF8AQQBWAEcAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAcwB1AG0AXwB2AGEAbABzACwAIABTAFUATQAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAcwB1AG0AXwB2AGEAbABzACAAPQAgADAALAAgAE4AQQAoACkALAAgAFMAVQBNAFAAUgBPAEQAVQBDAFQAKAByAGEAbgBnAGUALAAgAHIAYQBuAGcAZQApACAALwAgAHMAdQBtAF8AdgBhAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFIAQQBOAEcARQBfAFAARQBSAEMARQBOAFQAXwBUAFIAQQBOAFMARgBFAFIAOgBcAG4AXABuAFQAcgBhAG4AcwBmAGUAcgBzACAAYQAgAHAAZQByAGMAZQBuAHQAYQBnAGUAIABiAGUAdAB3AGUAZQBuACAAdAB3AG8AIABwAGEAaQByAHMAIABvAGYAIABuAHUAbQBiAGUAcgBzAFwAbgBcAG4ARQAuAGcALgAgAFAARQBSAEMARQBOAFQAXwBPAEYAXwBMAEkAUwBUAF8AWABGAFIAKAAzACwAMQAxACwANQAsADIALAAxADkAKQAgAD0AIAA2AC4AMgA1ACwAIAB3AGgAaQBjAGgAIABpAHMAOgBcAG4AIAAgACAAIABGAGkAbgBkACAAdABoAGUAIABwAGUAcgBjAGUAbgB0AGEAZwBlACAAcgBlAHAAcgBlAHMAZQBuAHQAZQBkACAAYgB5ACAANQAgAGIAZQB0AHcAZQBlAG4AIAAzACAAYQBuAGQAIAAxADEAXABuACAAIAAgACAARgBpAG4AZAAgAHQAaABlACAAbgB1AG0AYgBlAHIAIABiAGUAdAB3AGUAZQBuACAAMgAgAGEAbgBkACAAMQA5ACAAdwBoAGkAYwBoACAAYwBvAHIAcgBlAHMAcABvAG4AZABzACAAdABvAFwAbgAgACAAIAAgACAAIAAgACAAdABoAGEAdAAgAHMAYQBtAGUAIABwAGUAcgBjAGUAbgB0AGEAZwBlAC4AXABuAFwAbgAgACAAIAAgACAAIAAgACAAaQAuAGUALgAgADUAIABpAHMAIAAyADUAJQAgAG8AZgAgAHQAaABlACAAcgBhAG4AZwBlACAAMwAgAHQAbwAgADEAMQA7AFwAbgAgACAAIAAgACAAIAAgACAANgAuADIANQAgAGkAcwAgADIANQAlACAAbwBmACAAdABoAGUAIAByAGEAbgBnAGUAIAAyACAAdABvACAAMQA5AFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AUwBUAEEAVABfAFIAQQBOAEcARQBfAFAARQBSAEMARQBOAFQAXwBUAFIAQQBOAFMARgBFAFIAIAA9ACAATABBAE0AQgBEAEEAKABTAHQAYQByAHQATQBpAG4ALAAgAFMAdABhAHIAdABNAGEAeAAsACAAVABhAHIAZwBlAHQALAAgAEUAbgBkAE0AaQBuACwAIABFAG4AZABNAGEAeAAsACAAWwBkAGUAYwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGMAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBwAHIAZQBjACkALAAgADEANQAsACAAZABlAGMAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABwAGMAdAAsACAAKABUAGEAcgBnAGUAdAAgAC0AIABTAHQAYQByAHQATQBpAG4AKQAgAC8AIAAoAFMAdABhAHIAdABNAGEAeAAgAC0AIABTAHQAYQByAHQATQBpAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAYwBhAGwAYwAsACAAcABjAHQAIAAqACAAKABFAG4AZABNAGEAeAAgAC0AIABFAG4AZABNAGkAbgApACAAKwAgAEUAbgBkAE0AaQBuACwAXABuACAAIAAgACAAIAAgACAAIAByAG8AdQBuAGQAKABjAGEAbABjACwAIABkAGUAYwBwAHIAZQBjACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFIAQQBOAEcARQBfAFAARQBSAEMARQBOAFQAXwBPAEYAXwBWAEEATABVAEUAOgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHAAZQByAGMAZQBuAHQAYQBnAGUAIAAoAGEAcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACkAIABiAGUAdAB3AGUAZQBuACAAbQBpAG4AIABhAG4AZAAgAG0AYQB4AFwAbgAgACAAIAAgAHcAaABpAGMAaAAgAGkAcwAgAHIAZQBwAHIAZQBzAGUAbgB0AGUAZAAgAGIAeQAgAGEAIABnAGkAdgBlAG4AIAB2AGEAbAB1AGUAXABuAFwAbgBFAC4AZwAuACAAVABoAGUAIAB2AGEAbAB1AGUAIAA3ACAAcgBlAHAAcgBlAHMAZQBuAHQAcwAgADAALgA0ADQANAA0ADQALgAuAC4AIAAoADQANAAuADQAJQApACAAbwBmACAAdABoAGUAIAByAGEAbgBnAGUAIAAzACAAdABvACAAMQAyAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AUwBUAEEAVABfAFIAQQBOAEcARQBfAFAARQBSAEMARQBOAFQAXwBPAEYAXwBWAEEATABVAEUAIAA9ACAATABBAE0AQgBEAEEAKABtAGkAbgAsACAAbQBhAHgALAAgAHYAYQBsAHUAZQAsACAAWwBkAGUAYwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGMAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBwAHIAZQBjACkALAAgADEANQAsACAAZABlAGMAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABjAGEAbABjACwAIAAoAHYAYQBsAHUAZQAgAC0AIABtAGkAbgApACAALwAgACgAbQBhAHgAIAAtACAAbQBpAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkACgAYwBhAGwAYwAsACAAZABlAGMAcAByAGUAYwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBSAEEATgBHAEUAXwBWAEEATABVAEUAXwBPAEYAXwBQAEUAUgBDAEUATgBUADoAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB2AGEAbAB1AGUAIAB3AGgAaQBjAGgAIABpAHMAIAB0AGgAZQAgAGcAaQB2AGUAbgAgAHAAZQByAGMAZQBuAHQAYQBnAGUAIABiAGUAdAB3AGUAZQBuACAATQBJAE4AIABhAG4AZAAgAE0AQQBYAFwAbgBwAGMAdAAgAGkAcwAgAHMAdQBwAHAAbABpAGUAZAAgAGEAcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAbgB1AG0AYgBlAHIAIABiAGUAdAB3AGUAZQBuACAAMAAgAGEAbgBkACAAMQAwADAAXABuACAAIAAgACAAYQBuAGQAIABjAG8AbgB2AGUAcgB0AGUAZAAgAGkAbgB0AGUAcgBuAGEAbABsAHkAIAB0AG8AIABhACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgBcAG4AIAAgACAAIABpAC4AZQAuACAAcABjAHQAIAA9ACAANAAwAC4ANgA1ACAALQA+ACAAMAAuADQAMAA2ADUAXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBSAEEATgBHAEUAXwBWAEEATABVAEUAXwBPAEYAXwBQAEUAUgBDAEUATgBUACAAPQAgAEwAQQBNAEIARABBACgAbQBpAG4ALAAgAG0AYQB4ACwAIABwAGMAdAAsACAAWwBkAGUAYwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGMAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBwAHIAZQBjACkALAAgADEANQAsACAAZABlAGMAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABwAGMAdAAsACAAcABjAHQAIAAvACAAMQAwADAALABcAG4AIAAgACAAIAAgACAAIAAgAGMAYQBsAGMALAAgAHAAYwB0ACAAKgAgACgAbQBhAHgAIAAtACAAbQBpAG4AKQAgACsAIABtAGkAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkACgAYwBhAGwAYwAsACAAZABlAGMAcAByAGUAYwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFMAVABBAFQAXwBCAEUATgBGAE8AUgBEAF8ARABJAFMAVAAgAD0AIABMAEEATQBCAEQAQQAoAFsAbgB1AGwAbABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAaQBzAHQALAAgAFQATwBDAE8ATAAoAHsAMQAsACAAMgAsACAAMwAsACAANAAsACAANQAsACAANgAsACAANwAsACAAOAAsACAAOQB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0ACwAIABCAFkAUgBPAFcAKABsAGkAcwB0ACwAIABMAEEATQBCAEQAQQAoAHgALAAgAEwATwBHACgAMQAgACsAIAAoADEAIAAvACAATQBPAEQAKAB4ACwAIAAxADAAKQApACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBTAFQAQQBUAF8AUgBOAEQAXwBCAEUATgBGAE8AUgBEAF8AUwBJAE4ARwBMAEUAIAA9ACAATABBAE0AQgBEAEEAKABbAG4AdQBsAGwAXQAsAFwAbgAgACAAIAAgAFwAbgAgACAAIAAgAC8ALwAgAGcAZQBuAGUAcgBhAHQAZQBzACAAYQAgAHMAaQBuAGcAbABlACAAZABpAGcAaQB0ACAAdwBpAHQAaAAgAGEAIABwAHIAbwBiAGEAYgBpAGwAaQB0AHkAIABiAGEAcwBlAGQAIABvAG4AIAB0AGgAZQAgAEIAZQBuAGYAbwByAGQAIABEAGkAcwB0AHIAaQBiAHUAdABpAG8AbgBcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAbgB1AG0AbABpAHMAdAAsACAAUwBFAFEAVQBFAE4AQwBFACgAOQAsACAALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAG8AYgBsAGkAcwB0ACwAIAB7ADAALgAzADAAMQAsACAAMAAuADQANwA3ACwAIAAwAC4ANgAwADIALAAgADAALgA2ADkAOQAsACAAMAAuADcANwA4ACwAIAAwAC4AOAA0ADUALAAgADAALgA5ADAAMwAsACAAMAAuADkANQA0ACwAIAAxAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBvAGIALAAgAFgATABPAE8ASwBVAFAAKABSAEEATgBEACgAKQAsACAAcAByAG8AYgBsAGkAcwB0ACwAIABwAHIAbwBiAGwAaQBzAHQALAAgACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBvAGIAXwBpAG4AZABlAHgALAAgAE0AQQBUAEMASAAoAHAAcgBvAGIALAAgAHAAcgBvAGIAbABpAHMAdAAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIABkAGkAZwBpAHQALAAgAEkATgBEAEUAWAAoAG4AdQBtAGwAaQBzAHQALAAgAHAAcgBvAGIAXwBpAG4AZABlAHgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgAZABpAGcAaQB0ACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AUwBUAEEAVABfAFIATgBEAF8AQgBFAE4ARgBPAFIARAAgAD0AIABMAEEATQBCAEQAQQAoAFsAZABpAGcAaQB0AHMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkAGkAZwBpAHQAcwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGkAZwBpAHQAcwApACwAIAAzACwAIABkAGkAZwBpAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIABuAHUAbQBsAGkAcwB0ACwAIABTAEUAUQBVAEUATgBDAEUAKAA5ACwAIAAxACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBvAGIAbABpAHMAdAAsACAAewAwAC4AMwAwADEALAAgADAALgA0ADcANwAsACAAMAAuADYAMAAyACwAIAAwAC4ANgA5ADkALAAgADAALgA3ADcAOAAsACAAMAAuADgANAA1ACwAIAAwAC4AOQAwADMALAAgADAALgA5ADUANAAsACAAMQB9ACwAXABuACAAIAAgACAAIAAgACAAIAByAGEAbgBkAG8AbQBfAG4AdQBtAGIAZQByAHMALAAgAFIAQQBOAEQAQQBSAFIAQQBZACgAZABpAGcAaQB0AHMALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwBlAG4AZQByAGEAdABlAGQAXwBkAGkAZwBpAHQAcwAsACAASQBOAEQARQBYACgAbgB1AG0AbABpAHMAdAAsACAATQBBAFQAQwBIACgAWABMAE8ATwBLAFUAUAAoAHIAYQBuAGQAbwBtAF8AbgB1AG0AYgBlAHIAcwAsACAAcAByAG8AYgBsAGkAcwB0ACwAIABwAHIAbwBiAGwAaQBzAHQALAAgACwAIAAxACkALAAgAHAAcgBvAGIAbABpAHMAdAAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGcAZQBuAGUAcgBhAHQAZQBkAF8AbgB1AG0AYgBlAHIALAAgAFQARQBYAFQASgBPAEkATgAoAFwAIgBcACIALAAgAFQAUgBVAEUALAAgAGcAZQBuAGUAcgBhAHQAZQBkAF8AZABpAGcAaQB0AHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgAZwBlAG4AZQByAGEAdABlAGQAXwBuAHUAbQBiAGUAcgApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAC8ALwAgAEIAUgBBAEMASwBFAFQAUwBfAFQAQQBSAEcARQBUACAAPQAgAEwAQQBNAEIARABBACgAVABlAHMAdABBAHIAcgBhAHkALAAgAFQAYQByAGcAZQB0ACwAIABbAGkAbgBjAGwAXQAsACAAWwBtAG8AZABlAF0ALAAgAFsAZABlAGMAcAByAGUAYwBdACwAXABuAC8ALwAgACAAIAAgACAATABFAFQAKABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAGQAZQBjAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAZABlAGMAcAByAGUAYwApACwAIAAzACwAIABkAGUAYwBwAHIAZQBjACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALAAgAEkARgAoAE8AUgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABtAG8AZABlACAAPgAgADIAKQAsACAAMAAsACAAbQBvAGQAZQApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABpAG4AYwBsACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAGkAbgBjAGwAKQAsACAAaQBuAGMAbAAgAD4AIAAxACkALAAgADAALAAgAGkAbgBjAGwAKQAsAFwAbgBcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABiAHIAYQBjAGsAZQB0AGkAbgBnACAAdgBhAGwAdQBlAHMAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABsAG8AdwBlAHIALAAgAE0AQQBYACgARgBJAEwAVABFAFIAKABUAGUAcwB0AEEAcgByAGEAeQAsACAAVABlAHMAdABBAHIAcgBhAHkAIAA8ACAAVABhAHIAZwBlAHQAKQApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIAB1AHAAcABlAHIALAAgAE0ASQBOACgARgBJAEwAVABFAFIAKABUAGUAcwB0AEEAcgByAGEAeQAsACAAVABlAHMAdABBAHIAcgBhAHkAIAA+ACAAVABhAHIAZwBlAHQAKQApACwAXABuAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAbwB1AHQATABpAHMAdAAsACAASQBGACgAaQBuAGMAbAAgAD0AIAAwACwAIAB7AGwAbwB3AGUAcgAsACAAVABhAHIAZwBlAHQALAAgAHUAcABwAGUAcgB9ACwAIAB7AGwAbwB3AGUAcgAsACAAdQBwAHAAZQByAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIABUAE8AQwBPAEwAKABSAE8AVQBOAEQAKABvAHUAdABMAGkAcwB0ACwAIABkAGUAYwBwAHIAZQBjACkAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIABUAE8AUgBPAFcAKABSAE8AVQBOAEQAKABvAHUAdABMAGkAcwB0ACwAIABkAGUAYwBwAHIAZQBjACkAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIABcACIAKABcACIAIAAmACAAVABFAFgAVABKAE8ASQBOACgAXAAiACAAOgAgAFwAIgAsACAALAAgAEYASQBYAEUARAAoAG8AdQB0AEwAaQBzAHQALAAgAGQAZQBjAHAAcgBlAGMAKQApACAAJgAgAFwAIgApAFwAIgBcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4ALwAvACAAIAAgACAAIAApAFwAbgAvAC8AIAApADsAXABuAFwAbgAvAC8AIABCAFIAQQBDAEsARQBUAFMAXwBBAFIAUgBBAFkAIAA9ACAATABBAE0AQgBEAEEAKABMAG8AbwBrAHUAcABBAHIAcgBhAHkALAAgAFIAZQB0AHUAcgBuAEEAcgByAGEAeQAsACAAWwBNAG8AZABlAF0ALABcAG4ALwAvACAAIAAgACAAIABMAEUAVAAoAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgATwBSACgASQBTAE8ATQBJAFQAVABFAEQAKABNAG8AZABlACkALAAgAE0AbwBkAGUAIAA+ACAAMgApACwAIAAwACwAIABNAG8AZABlACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAEEAdgBnACwAIABBAFYARQBSAEEARwBFACgATABvAG8AawB1AHAAQQByAHIAYQB5ACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAEwAZQBhAHMAdAAsACAATQBBAFgAKABGAEkATABUAEUAUgAoAEwAbwBvAGsAdQBwAEEAcgByAGEAeQAsACAATABvAG8AawB1AHAAQQByAHIAYQB5ACAAPAAgAEEAdgBnACkAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAATQBvAHMAdAAsACAATQBJAE4AKABGAEkATABUAEUAUgAoAEwAbwBvAGsAdQBwAEEAcgByAGEAeQAsACAATABvAG8AawB1AHAAQQByAHIAYQB5ACAAPgAgAEEAdgBnACkAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAATABlAGEAcwB0AF8AaQBuAGQAZQB4ACwAIABYAEwATwBPAEsAVQBQACgATABlAGEAcwB0ACwAIABMAG8AbwBrAHUAcABBAHIAcgBhAHkALAAgAFIAZQB0AHUAcgBuAEEAcgByAGEAeQApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABNAG8AcwB0AF8AaQBuAGQAZQB4ACwAIABYAEwATwBPAEsAVQBQACgATQBvAHMAdAAsACAATABvAG8AawB1AHAAQQByAHIAYQB5ACwAIABSAGUAdAB1AHIAbgBBAHIAcgBhAHkAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAbABpAHMAdAAsACAAVABFAFgAVABKAE8ASQBOACgAXAAiACAAXAAiACwAIAAsACAATABlAGEAcwB0AF8AaQBuAGQAZQB4ACwAIABBAHYAZwAsACAATQBvAHMAdABfAGkAbgBkAGUAeAApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIABUAE8AQwBPAEwAKABUAEUAWABUAFMAUABMAEkAVAAoAGwAaQBzAHQALAAgAFwAIgAgAFwAIgApACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAVABPAFIATwBXACgAVABFAFgAVABTAFAATABJAFQAKABsAGkAcwB0ACwAIABcACIAIABcACIAKQApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgAEMATwBOAEMAQQBUACgAXAAiACgAXAAiACwAIABUAEUAWABUAEoATwBJAE4AKABcACIAIAA6ACAAXAAiACwAIAAsACAARgBJAFgARQBEACgATABlAGEAcwB0ACwAIAAzACkALAAgAEYASQBYAEUARAAoAEEAdgBnACwAIAAzACkALAAgAEYASQBYAEUARAAoAE0AbwBzAHQALAAgADMAKQApACwAIABcACIAKQBcACIAKQBcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAvAC8AIAAgACAAIAAgACkAXABuAC8ALwAgACkAOwAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAiACwAIgBTAFQAQQBUAF8AUwBUAEQARQBSAFIAIgAsACIAUwBUAEEAVABfAE0ASQBOAE0AQQBYACIALAAiAFMAVABBAFQAXwBTAFUATQBNAEEAUgBZACIALAAiAFMAVABBAFQAXwBHAEUATwA1ACIALAAiAFMAVABBAFQAXwBWAE8ATABVAE0ARQAiACwAIgBTAFQAQQBUAF8AUwBIAEEAUABFACIALAAiAFMAVABBAFQAXwBNAEkARABSAEEATgBHAEUAIgAsACIAUwBUAEEAVABfAEYAUgBFAFEAXwBUAEEAQgBMAEUAIgAsACIAUwBUAEEAVABfAFcAVABEAF8AQQBWAEcAIgAsACIAUwBUAEEAVABfAFMARQBMAEYAXwBXAFQARABfAEEAVgBHACIALAAiAFMAVABBAFQAXwBTAFQAQQBUAF8AUgBBAE4ARwBFAF8AUABFAFIAQwBFAE4AVABfAFQAUgBBAE4AUwBGAEUAUgAiACwAIgBTAFQAQQBUAF8AUwBUAEEAVABfAFIAQQBOAEcARQBfAFAARQBSAEMARQBOAFQAXwBPAEYAXwBWAEEATABVAEUAIgAsACIAUwBUAEEAVABfAFIAQQBOAEcARQBfAFYAQQBMAFUARQBfAE8ARgBfAFAARQBSAEMARQBOAFQAIgAsACIAUwBUAEEAVABfAEIARQBOAEYATwBSAEQAXwBEAEkAUwBUACIALAAiAFMAVABBAFQAXwBSAE4ARABfAEIARQBOAEYATwBSAEQAXwBTAEkATgBHAEwARQAiACwAIgBTAFQAQQBUAF8AUgBOAEQAXwBCAEUATgBGAE8AUgBEACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIAWQBNAEQAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAXABuAFMAVABBAFQAXwBRAE4AVABJAEwARQBTAFwAbgBSAGUAdAB1AHIAbgBzACAAZQBxAHUAYQBsAGwAeQAgAHMAcABhAGMAZQBkACAAcQB1AGEAbgB0AGkAbABlAHMAIABmAHIAbwBtACAAYQAgAG4AdQBtAGUAcgBpAGMAIAByAGEAbgBnAGUALAAgAHcAaQB0AGgAIABvAHAAdABpAG8AbgBhAGwAIABsAGEAYgBlAGwAcwAgAGEAbgBkACAAYgBpAG4ALQBzAHQAeQBsAGUAIABzAGwAaQBjAGkAbgBnAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAIAAgACAAIAAgACAAFCAgAE4AdQBtAGUAcgBpAGMAIABpAG4AcAB1AHQAIAByAGEAbgBnAGUAIAAoAGUALgBnAC4ALAAgAEEAMQA6AEEAMQAwADAAKQBcAG4ALQAgAFsAZABpAHYAaQBzAGkAbwBuAHMAXQAgABQgIAAoAG8AcAB0AGkAbwBuAGEAbAApACAATgB1AG0AYgBlAHIAIABvAGYAIABxAHUAYQBuAHQAaQBsAGUAIABpAG4AdABlAHIAdgBhAGwAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAxADAAKQBcAG4ALQAgAFsAbQBvAGQAZQBdACAAIAAgACAAIAAgABQgIAAoAG8AcAB0AGkAbwBuAGEAbAApACAAVQBzAGUAIABcACIATABCAEwAXAAiACAAdABvACAAcgBlAHQAdQByAG4AIABsAGEAYgBlAGwAZQBkACAAMgAtAGMAbwBsAHUAbQBuACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAdgBhAGwAdQBlAHMAIABvAG4AbAB5ACkAXABuAC0AIABbAHMAdAB5AGwAZQBdACAAIAAgACAAIAAUICAAKABvAHAAdABpAG8AbgBhAGwAKQAgAFwAIgBBAEwATABcACIAIAAoAGQAZQBmAGEAdQBsAHQAKQAgAGkAbgBjAGwAdQBkAGUAcwAgADAAJQAgAGEAbgBkACAAMQAwADAAJQA7ACAAXAAiAEIASQBOAFwAIgAgAGUAeABjAGwAdQBkAGUAcwAgAGIAbwB0AGgAIABiAG8AdQBuAGQAYQByAGkAZQBzAFwAbgAtACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACAAFCAgACgAbwBwAHQAaQBvAG4AYQBsACkAIABEAGUAYwBpAG0AYQBsACAAcgBvAHUAbgBkAGkAbgBnACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIABxAHUAYQBuAHQAaQBsAGUAIAB2AGEAbAB1AGUAcwAsACAAbwByACAAYQAgADIALQBjAG8AbAB1AG0AbgAgAGwAYQBiAGUAbABlAGQAIABhAHIAcgBhAHkALAAgAGQAZQBwAGUAbgBkAGkAbgBnACAAbwBuACAAbQBvAGQAZQAuAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzADoAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAARABlAGMAaQBsAGUAcwBcAG4ALQAgAFMAVABBAFQAXwBRAE4AVABJAEwARQBTACgAQQAxADoAQQAxADAAMAAsACAANAAsACAAXAAiAEwAQgBMAFwAIgApACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAUQB1AGEAcgB0AGkAbABlAHMAIAB3AGkAdABoACAAbABhAGIAZQBsAHMAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAALAAgADEAMAAsACAALAAgAFwAIgBCAEkATgBcACIAKQAgACAAIAAgACAAIAAgACAAkiEgAEkAbgB0AGUAcgBuAGEAbAAgAGIAaQBuACAAYgBvAHUAbgBkAGEAcgBpAGUAcwAgACgAMQAwAC0AdABpAGwAZQBzACkAXABuAC0AIABTAFQAQQBUAF8AUQBOAFQASQBMAEUAUwAoAEEAMQA6AEEAMQAwADAALAAgADIAMAAsACAAXAAiAEwAQgBMAFwAIgAsACAAXAAiAEIASQBOAFwAIgAsACAAMgApACAAkiEgAEwAYQBiAGUAbABlAGQAIABiAGkAbgAgAGMAdQB0AHMAIAB3AGkAdABoACAAMgAtAGQAaQBnAGkAdAAgAHIAbwB1AG4AZABpAG4AZwBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFEATgBUAEkATABFAFMAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAZABpAHYAaQBzAGkAbwBuAHMAXQAsACAAWwBtAG8AZABlAF0ALAAgAFsAcwB0AHkAbABlAF0ALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABOAG8AcgBtAGEAbABpAHoAZQAgAG8AcAB0AGkAbwBuAGEAbAAgAGEAcgBnAHUAbQBlAG4AdABzAFwAbgAgACAAIAAgACAAIAAgACAAZABpAHYAaQBzAGkAbwBuAHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAZABpAHYAaQBzAGkAbwBuAHMAKQAsACAAMQAwACwAIABkAGkAdgBpAHMAaQBvAG4AcwApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbQBvAGQAZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAHMAdAB5AGwAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABzAHQAeQBsAGUAKQAsACAAXAAiAEEATABMAFwAIgAsACAAVQBQAFAARQBSACgAcwB0AHkAbABlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwBpAHMAaQBvAG4AKQAsACAAMwAsACAAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFYAYQBsAGkAZABhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIABjAG8AdQBuAHQAVgBhAGwAcwAsACAAQwBPAFUATgBUACgAcgBhAG4AZwBlACkALABcAG4AIAAgACAAIAAgACAAIAAgAGkAcwBWAGEAbABpAGQALAAgAEkAUwBOAFUATQBCAEUAUgAoAGQAaQB2AGkAcwBpAG8AbgBzACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAGMAbwB1AG4AdABWAGEAbABzACAAPQAgADAALAAgAFMAUQBSAFQAKABcACIAYQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABPAFIAKABOAE8AVAAoAGkAcwBWAGEAbABpAGQAKQAsACAAZABpAHYAaQBzAGkAbwBuAHMAIAA8ACAAMQApACwAIABTAFEAUgBUACgALQAxACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFAAZQByAGMAZQBuAHQAaQBsAGUAIABjAHUAdAAgAHAAbwBpAG4AdABzACAAYgBhAHMAZQBkACAAbwBuACAAcwB0AHkAbABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcABjAHQAaQBsAGUAcwAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcwB0AHkAbABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBCAEkATgBcACIALAAgAFMARQBRAFUARQBOAEMARQAoAGQAaQB2AGkAcwBpAG8AbgBzACAALQAgADEALAAgADEALAAgADEAKQAgAC8AIABkAGkAdgBpAHMAaQBvAG4AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKABkAGkAdgBpAHMAaQBvAG4AcwAgACsAIAAxACwAIAAxACwAIAAwACkAIAAvACAAZABpAHYAaQBzAGkAbwBuAHMAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIAA9ACAAQQBMAEwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAATABhAGIAZQBsACAAZgBvAHIAbQBhAHQAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHAAYwB0AF8AbABhAGIAZQBsAHMALAAgAFQARQBYAFQAKABwAGMAdABpAGwAZQBzACwAIABcACIAMAAlAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQwBhAGwAYwB1AGwAYQB0AGUAIABxAHUAYQBuAHQAaQBsAGUAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHAAYwB0AF8AdgBhAGwAcwAsACAAUgBPAFUATgBEACgAUABFAFIAQwBFAE4AVABJAEwARQAuAEkATgBDACgAcgBhAG4AZwBlACwAIABwAGMAdABpAGwAZQBzACkALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AHQAaQBuAGcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBMAEIATABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAKAB7ADEALAAgADIAfQAsACAAcABjAHQAXwBsAGEAYgBlAGwAcwAsACAAVgBBAEwAVQBFACgAcABjAHQAXwB2AGEAbABzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAE8AQwBPAEwAKABwAGMAdABfAHYAYQBsAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBTAFQARABFAFIAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHMAdABhAG4AZABhAHIAZAAgAGUAcgByAG8AcgAgAG8AZgAgAHQAaABlACAAbQBlAGEAbgAgACgAUwBFAE0AKQAgAGYAbwByACAAYQAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIABhAHIAcgBhAHkAIAAgACAAIAAgAD0AIABUAGgAZQAgAGQAYQB0AGEAcwBlAHQAIAB0AG8AIABlAHYAYQBsAHUAYQB0AGUAXABuAC0AIABtAG8AZABlACAAIAAgACAAIAAgAD0AIABPAHAAdABpAG8AbgBhAGwAOwAgAFwAIgBwAG8AcABcACIAIABmAG8AcgAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAKQAsACAAXAAiAHMAYQBtAHAAXAAiACAAZgBvAHIAIABzAGEAbQBwAGwAZQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAEwAQgBMAFwAIgAgAHQAbwAgAHIAZQB0AHUAcgBuACAAYQAgAGwAYQBiAGUAbABlAGQAIABzAHQAcgBpAG4AZwAsACAAbwB0AGgAZQByAHcAaQBzAGUAIAByAGUAdAB1AHIAbgBzACAAbgB1AG0AZQByAGkAYwBcAG4ALQAgAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAG8AdQBuAGQAIAByAGUAcwB1AGwAdAAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4ATgBvAHQAZQBzADoAXABuAC0AIABTAHQAYQBuAGQAYQByAGQAIABlAHIAcgBvAHIAIAByAGUAZgBsAGUAYwB0AHMAIAB0AGgAZQAgAGUAeABwAGUAYwB0AGUAZAAgAHYAYQByAGkAYQBiAGkAbABpAHQAeQAgAG8AZgAgAHQAaABlACAAcwBhAG0AcABsAGUAIABtAGUAYQBuACwAIABhAHMAcwB1AG0AaQBuAGcAIAB0AGgAZQAgAGQAYQB0AGEAIAByAGUAcAByAGUAcwBlAG4AdABzACAAYQAgAHIAYQBuAGQAbwBtACAAcwBhAG0AcABsAGUALgBcAG4ALQAgAEkAZgAgAHQAaABlACAAZABhAHQAYQBzAGUAdAAgAHIAZQBwAHIAZQBzAGUAbgB0AHMAIAB0AGgAZQAgAGUAbgB0AGkAcgBlACAAcABvAHAAdQBsAGEAdABpAG8AbgAsACAAUwBFAE0AIABpAHMAIABtAGEAdABoAGUAbQBhAHQAaQBjAGEAbABsAHkAIAB2AGEAbABpAGQAIABiAHUAdAAgAG4AbwB0ACAAcAByAGEAYwB0AGkAYwBhAGwAbAB5ACAAbgBlAGMAZQBzAHMAYQByAHkAFCBpAHQAIABtAG8AZABlAGwAcwAgAGUAcgByAG8AcgAgAHQAaABhAHQAIABkAG8AZQBzAG4AGSB0ACAAZQB4AGkAcwB0AC4AXABuAFwAbgBFAHgAYQBtAHAAbABlADoAXABuAD0AUwBUAEEAVABfAFMAVABEAEUAUgBSACgAQQAxADoAQQAxADAAMAAsACAAXAAiAHMAYQBtAHAAXAAiACwAIABcACIATABCAEwAXAAiACwAIAAyACkAXABuAJIhIABcACIAUwB0AGEAbgBkAGEAcgBkACAARQByAHIAbwByADoAIAAxAC4AMgA3AFwAIgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFMAVABEAEUAUgBSACAAPQAgAEwAQQBNAEIARABBACgAYQByAHIAYQB5ACwAIABbAG0AbwBkAGUAXQAsACAAWwBsAGEAYgBlAGwAXQAsACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMAaQBzAGkAbwBuACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAaQBzAGkAbwBuACkALAAgADMALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAbABhAGIAZQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABcACIAcABvAHAAXAAiACwAIABMAE8AVwBFAFIAKABtAG8AZABlACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABzAHQAYQBuAGQAYQByAGQAIABlAHIAcgBvAHIAIABiAGEAcwBlAGQAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAAcwB0AGQAZQByAHIALAAgAFMAVwBJAFQAQwBIACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAHAAbwBwAFwAIgAsACAAUwBUAEQARQBWAC4AUAAoAGEAcgByAGEAeQApACAALwAgAFMAUQBSAFQAKABDAE8AVQBOAFQAQQAoAGEAcgByAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAHMAYQBtAHAAXAAiACwAIABTAFQARABFAFYALgBTACgAYQByAHIAYQB5ACkAIAAvACAAUwBRAFIAVAAoAEMATwBVAE4AVABBACgAYQByAHIAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAFQARABFAFYALgBQACgAYQByAHIAYQB5ACkAIAAvACAAUwBRAFIAVAAoAEMATwBVAE4AVABBACgAYQByAHIAYQB5ACkAKQAgACAALwAvACAAZgBhAGwAbABiAGEAYwBrAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABSAE8AVQBOAEQAKABzAHQAZABlAHIAcgAsACAAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIAbABiAGwAXAAiACwAIABcACIAUwB0AGEAbgBkAGEAcgBkACAARQByAHIAbwByADoAIABcACIAIAAmACAAcgBlAHMAdQBsAHQALAAgAHIAZQBzAHUAbAB0ACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8ATQBJAE4ATQBBAFgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABtAGkAbgBpAG0AdQBtACAAYQBuAGQAIABtAGEAeABpAG0AdQBtACAAbwBmACAAYQAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkALAAgAG8AcAB0AGkAbwBuAGEAbABsAHkAIABsAGEAYgBlAGwAZQBkACAAYQBzACAAYQAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AIABhAHIAcgBhAHkALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIABhAHIAcgBhAHkAIAAgAD0AIABUAGgAZQAgAGQAYQB0AGEAcwBlAHQAIAB0AG8AIABlAHYAYQBsAHUAYQB0AGUAXABuAC0AIABwAHIAZQBjACAAIAAgAD0AIABPAHAAdABpAG8AbgBhAGwAOwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAdABvACAAcgBvAHUAbgBkACAAcgBlAHMAdQBsAHQAIAAoAGQAZQBmAGEAdQBsAHQAOgAgADMAKQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAEwAQgBMAFwAIgAgAHIAZQB0AHUAcgBuAHMAIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAbwB1AHQAcAB1AHQAIAB3AGkAdABoACAAdABlAHgAdAAgAGEAbgBkACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQBzAFwAbgAtACAAbABhAHkAbwB1AHQAIAA9ACAATwBwAHQAaQBvAG4AYQBsADsAIABcACIASABcACIAIABmAG8AcgAgAGgAbwByAGkAegBvAG4AdABhAGwALAAgAFwAIgBWAFwAIgAgAGYAbwByACAAdgBlAHIAdABpAGMAYQBsACAAKABkAGUAZgBhAHUAbAB0ADoAIABcACIAVgBcACIAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAEQAZQBmAGEAdQBsAHQAOgAgAHsAbQBpAG4AOwAgAG0AYQB4AH0AIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AFwAbgAtACAASQBmACAAbABhAGIAZQBsACAAPQAgAFwAIgBMAEIATABcACIAOgAgAFwAbgAgACAAIAAgAE0AaQBuACAAIAAgACAAIAB8ACAAdgBhAGwAdQBlACAAIABcAG4AIAAgACAAIABNAGEAeAAgACAAIAAgACAAfAAgAHYAYQBsAHUAZQAgACAAXABuAC0AIABMAGEAeQBvAHUAdAAgAG0AbwBkAGUAIABhAGYAZgBlAGMAdABzACAAbwByAGkAZQBuAHQAYQB0AGkAbwBuACAAbwBuAGwAeQAgAGkAZgAgAGwAYQBiAGUAbAAgAGAiIABcACIATABCAEwAXAAiAFwAbgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAE0ASQBOAE0AQQBYACAAPQAgAEwAQQBNAEIARABBACgAYQByAHIAYQB5ACwAIABbAHAAcgBlAGMAXQAsACAAWwBsAGEAYgBlAGwAXQAsACAAWwBsAGEAeQBvAHUAdABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbABhAHkAbwB1AHQALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbABhAHkAbwB1AHQAKQAsACAAXAAiAFYAXAAiACwAIABVAFAAUABFAFIAKABsAGEAeQBvAHUAdAApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABSAE8AVQBOAEQAKABNAEkATgAoAGEAcgByAGEAeQApACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AYQB4AF8AdgBhAGwALAAgAFIATwBVAE4ARAAoAE0AQQBYACgAYQByAHIAYQB5ACkALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AF8AbABiAGwALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAbQBpAG4AXwB2AGEAbAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAE0AYQB4AFwAIgAsACAAbQBhAHgAXwB2AGEAbAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AF8AcgBhAHcALAAgAEkARgAoAGwAYQB5AG8AdQB0ACAAPQAgAFwAIgBIAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAG0AaQBuAF8AdgBhAGwALAAgAG0AYQB4AF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAG0AaQBuAF8AdgBhAGwALAAgAG0AYQB4AF8AdgBhAGwAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABJAEYAKABsAGEAYgBlAGwAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAAcgBlAHMAdQBsAHQAXwBsAGIAbAAsACAAcgBlAHMAdQBsAHQAXwByAGEAdwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBTAFUATQBNAEEAUgBZAFwAbgBcAG4AUAByAG8AdgBpAGQAZQBzACAAYQAgAGMAbwBuAGMAaQBzAGUAIABzAHQAYQB0AGkAcwB0AGkAYwBhAGwAIABzAHUAbQBtAGEAcgB5ACAAZgBvAHIAIABhACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHIAYQBuAGcAZQAgACAAPQAgAFQAaABlACAAZABhAHQAYQBzAGUAdAAgAHQAbwAgAGUAdgBhAGwAdQBhAHQAZQBcAG4ALQAgAG0AbwBkAGUAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAXAAiAFMATQBSAFkAXAAiACAAbwByACAAXAAiAFMAUABBAE4AXAAiACAAKABkAGUAZgBhAHUAbAB0ADoAIABTAFAAQQBOACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIABTAE0AUgBZADoAIABNAGkAbgAsACAATQBlAGEAbgAsACAATQBlAGQAaQBhAG4ALAAgAE0AYQB4ACwAIABTAHQAZABlAHYAXABuACAAIAAgACAAIAAgACAAIAAgACAAIABTAFAAQQBOADoAIABNAGkAbgAsACAAvAMSIsMDLAAgAE0AZQBhAG4ALAAgALwDKwDDAywAIABNAGEAeAAsACAAUwB0AGQAZQB2AFwAbgAtACAAbABhAGIAZQBsACAAIAA9ACAATwBwAHQAaQBvAG4AYQBsADsAIABcACIATABCAEwAXAAiACAAcgBlAHQAdQByAG4AcwAgAGEAIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAbABhAGIAZQBsAGUAZAAgAGEAcgByAGEAeQBcAG4ALQAgAHAAcgBlAGMAIAAgACAAPQAgAE8AcAB0AGkAbwBuAGEAbAA7ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAAoAGQAZQBmAGEAdQBsAHQAOgAgADMAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAEEAIAB2AGUAcgB0AGkAYwBhAGwAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5ACAAbwByACAAbABhAGIAZQBsAGUAZAAgAG0AYQB0AHIAaQB4ACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlACAAYQBuAGQAIABsAGEAYgBlAGwAIABmAGwAYQBnAFwAbgBcAG4ATQBvAGQAZQAgAEQAZQBzAGMAcgBpAHAAdABpAG8AbgBzADoAXABuAC0AIABcACIAUwBNAFIAWQBcACIAOgAgAEIAYQBsAGEAbgBjAGUAZAAgAHMAbgBhAHAAcwBoAG8AdAAgAG8AZgAgAGMAZQBuAHQAZQByACAAYQBuAGQAIABzAHAAcgBlAGEAZABcAG4ALQAgAFwAIgBTAFAAQQBOAFwAIgA6ACAARQBtAHAAaABhAHMAaQB6AGUAcwAgAGQAaQBzAHQAcgBpAGIAdQB0AGkAbwBuACAAcwBoAGEAcABlACAAYQByAG8AdQBuAGQAIAB0AGgAZQAgAG0AZQBhAG4AIAAoALwDIACxACAAwwMpACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAdwBpAHQAaAAgAGMAbABlAGEAcgAgAGwAYQBiAGUAbABpAG4AZwAgAG8AZgAgAE0AZQBhAG4AIAAoALwDKQAgAGEAbgBkACAAUwB0AGQAZQB2ACAAKADDAykAIABvAG4AbAB5AFwAbgBcAG4AKgAvAFwAbgBcAG4AUwBUAEEAVABfAFMAVQBNAE0AQQBSAFkAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbQBvAGQAZQBdACwAIABbAGwAYQBiAGUAbABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAByAGEAdwBfAG0AbwBkAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABcACIAUwBQAEEATgBcACIALAAgAFUAUABQAEUAUgAoAG0AbwBkAGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKAByAGEAdwBfAG0AbwBkAGUAIAA9ACAAXAAiAFMATQBSAFkAXAAiACwAIAByAGEAdwBfAG0AbwBkAGUAIAA9ACAAXAAiAFMAUABBAE4AXAAiACkALAAgAHIAYQB3AF8AbQBvAGQAZQAsACAAMQAvADAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgALwDLAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAwwMsACAAUwBUAEQARQBWAC4AUAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABNAEkATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAIABNAEEAWAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGUAZABfAHYAYQBsACwAIABNAEUARABJAEEATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIAC8A18AbQBpAG4AdQBzAF8AwwMsACAAvAMgAC0AIADDAywAXABuACAAIAAgACAAIAAgACAAIAC8A18AcABsAHUAcwBfAMMDLAAgALwDIAArACAAwwMsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFMAdQBtAG0AYQByAHkAIABtAG8AZABlADoAIABNAGkAbgAsACAATQBlAGEAbgAsACAATQBlAGQAaQBhAG4ALAAgAE0AYQB4ACwAIABTAHQAZABlAHYAXABuACAAIAAgACAAIAAgACAAIABzAG0AcgB5AF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBpAG4AXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8AywAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AZQBkAF8AdgBhAGwALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBhAHgAXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIADDA1wAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcwBtAHIAeQBfAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBNAGkAbgBcACIALAAgAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIATQBlAGQAaQBhAG4AXAAiACwAIABcACIATQBhAHgAXAAiACwAIABcACIAUwB0AGQAZQB2ACAAKADDAykAXAAiACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABTAHAAYQBuACAAbQBvAGQAZQA6ACAATQBpAG4ALAAgALwDEiLDAywAIABNAGUAYQBuACwAIAC8AysAwwMsACAATQBhAHgALAAgAMMDXABuACAAIAAgACAAIAAgACAAIABzAHAAYQBuAF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbQBpAG4AXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8A18AbQBpAG4AdQBzAF8AwwMsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAC8AywAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgALwDXwBwAGwAdQBzAF8AwwMsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAMMDXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABzAHAAYQBuAF8AbABhAGIAZQBsAHMALAAgAFYAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAXAAiALwDIAASIiAAwwNcACIALAAgAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIAvAMgACsAIADDA1wAIgAsACAAXAAiAE0AYQB4AFwAIgAsACAAXAAiAFMAdABkAGUAdgAgACgAwwMpAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcwBlAGwAZQBjAHQAZQBkAF8AdgBhAGwAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAUwBQAEEATgBcACIALAAgAHMAcABhAG4AXwB2AGEAbABzACwAIABzAG0AcgB5AF8AdgBhAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIABzAGUAbABlAGMAdABlAGQAXwBsAGEAYgBlAGwAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAUwBQAEEATgBcACIALAAgAHMAcABhAG4AXwBsAGEAYgBlAGwAcwAsACAAcwBtAHIAeQBfAGwAYQBiAGUAbABzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwAsACAAUgBPAFUATgBEACgAcwBlAGwAZQBjAHQAZQBkAF8AdgBhAGwAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAcwBlAGwAZQBjAHQAZQBkAF8AbABhAGIAZQBsAHMALAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAEcARQBPADUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGcAZQBvAG0AZQB0AHIAaQBjACAAZgBpAHYAZQAtAHAAbwBpAG4AdAAgAHMAdQBtAG0AYQByAHkAIABvAGYAIABhACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAuAFwAbgBcAG4AVABoAGkAcwAgAGkAcwAgAE4ATwBUACAAYQAgAHAAZQByAGMAZQBuAHQAaQBsAGUALQBiAGEAcwBlAGQAIABzAHUAbQBtAGEAcgB5ACAAKABsAGkAawBlACAAcQB1AGEAcgB0AGkAbABlAHMAKQAsAFwAbgBiAHUAdAAgAGEAIABzAHkAbQBtAGUAdAByAGkAYwAgAHAAbwBzAGkAdABpAG8AbgBhAGwAIABzAGMAYQBmAGYAbwBsAGQAIABhAGMAcgBvAHMAcwAgAHQAaABlACAATQBpAG4AEyBNAGEAeAAgAHMAcABhAG4ALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIAByAGEAbgBnAGUAIAAgACAAOgAgAFIAZQBxAHUAaQByAGUAZAAgAGEAcgByAGEAeQAgAG8AZgAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAcwBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIAB1AHMAZQAgAFwAIgBMAEIATABcACIAIABmAG8AcgAgAGwAYQBiAGUAbABlAGQAIAAyAC0AYwBvAGwAdQBtAG4AIABvAHUAdABwAHUAdAAgACgAZABlAGYAYQB1AGwAdAA6ACAAdQBuAGwAYQBiAGUAbABlAGQAKQBcAG4ALQAgAHAAcgBlAGMAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAG4AdQBtAGUAcgBpAGMAIABhAHIAcgBhAHkAIABvAHIAIABsAGEAYgBlAGwAZQBkACAAbQBhAHQAcgBpAHgAIABpAG4AYwBsAHUAZABpAG4AZwA6AFwAbgAgACAAewBNAGkAbgAsACAATABvAHcAZQByACAATQBpAGQALAAgAE0AaQBkAHIAYQBuAGcAZQAsACAAVQBwAHAAZQByACAATQBpAGQALAAgAE0AYQB4AH0AXABuAFwAbgBGAG8AcgBtAHUAbABhAHMAOgBcAG4ALQAgAE0AaQBuACAAIAAgACAAIAAgACAAIAAgAD0AIABNAEkATgAoAHIAYQBuAGcAZQApAFwAbgAtACAATQBpAGQAcgBhAG4AZwBlACAAIAAgACAAPQAgACgATQBJAE4AIAArACAATQBBAFgAKQAgAC8AIAAyAFwAbgAtACAATABvAHcAZQByACAATQBpAGQAIAAgACAAPQAgACgATQBJAE4AIAArACAATQBpAGQAcgBhAG4AZwBlACkAIAAvACAAMgBcAG4ALQAgAFUAcABwAGUAcgAgAE0AaQBkACAAIAAgAD0AIAAoAE0AaQBkAHIAYQBuAGcAZQAgACsAIABNAEEAWAApACAALwAgADIAXABuAC0AIABNAGEAeAAgACAAIAAgACAAIAAgACAAIAA9ACAATQBBAFgAKAByAGEAbgBnAGUAKQBcAG4AXABuAE4AbwB0AGUAOgBcAG4ALQAgAFQAaABpAHMAIABmAHUAbgBjAHQAaQBvAG4AIABpAHMAIAAqACoAZABpAHMAdAByAGkAYgB1AHQAaQBvAG4ALQBhAGcAbgBvAHMAdABpAGMAKgAqAC4AIABJAHQAIAByAGUAcABvAHIAdABzACAAbgB1AG0AZQByAGkAYwAgAHAAbwBzAGkAdABpAG8AbgAgAG8AbgBsAHkALAAgAFwAbgAgACAAdwBpAHQAaABvAHUAdAAgAHIAZQBnAGEAcgBkACAAdABvACAAdABoAGUAIABmAHIAZQBxAHUAZQBuAGMAeQAgAG8AcgAgAGMAbAB1AHMAdABlAHIAaQBuAGcAIABvAGYAIAB2AGEAbAB1AGUAcwAuACAAVABoAGEAdAAgAG0AZQBhAG4AcwAgAGQAYQB0AGEAcwBlAHQAcwAgAFwAbgAgACAAdwBpAHQAaAAgAGgAaQBnAGgAbAB5ACAAcwBrAGUAdwBlAGQAIABvAHIAIAByAGUAcABlAHQAaQB0AGkAdgBlACAAdgBhAGwAdQBlAHMAIABtAGEAeQAgAHMAdABpAGwAbAAgAHkAaQBlAGwAZAAgAGUAdgBlAG4AbAB5ACAAcwBwAGEAYwBlAGQAIAByAGUAcwB1AGwAdABzACAAXABuACAAIABpAGYAIABNAGkAbgAgAGEAbgBkACAATQBhAHgAIAByAGUAbQBhAGkAbgAgAHQAaABlACAAcwBhAG0AZQAuACAASQB0ACAAaQBzACAAYgBlAHMAdAAgAHUAbgBkAGUAcgBzAHQAbwBvAGQAIABhAHMAIABhACAAKgBzAHkAbQBtAGUAdAByAHkAIABzAGMAYQBmAGYAbwBsAGQAKgAsACAAXABuACAAIABuAG8AdAAgAGEAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgBhAGwAIABhAG4AYQBsAHkAcwBpAHMALgBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBHAEUATwA1ACAAPQAgAEwAQQBNAEIARABBACgAcgBhAG4AZwBlACwAIABbAGwAYQBiAGUAbABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABsAGEAYgBlAGwALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbABhAGIAZQBsACkALAAgAFwAIgBcACIALAAgAFUAUABQAEUAUgAoAGwAYQBiAGUAbAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABtAGkAbgBfAHYAYQBsACwAIABNAEkATgAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHYAYQBsACwAIABNAEEAWAAoAHIAYQBuAGcAZQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGkAZAByAGEAbgBnAGUALAAgACgAbQBpAG4AXwB2AGEAbAAgACsAIABtAGEAeABfAHYAYQBsACkAIAAvACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAbABvAHcAZQByAF8AbQBpAGQALAAgACgAbQBpAG4AXwB2AGEAbAAgACsAIABtAGkAZAByAGEAbgBnAGUAKQAgAC8AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAB1AHAAcABlAHIAXwBtAGkAZAAsACAAKABtAGkAZAByAGEAbgBnAGUAIAArACAAbQBhAHgAXwB2AGEAbAApACAALwAgADIALABcAG4AXABuACAAIAAgACAAIAAgACAAIAByAGEAdwBfAHYAYQBsAHMALAAgAFYAUwBUAEEAQwBLACgAbQBpAG4AXwB2AGEAbAAsACAAbABvAHcAZQByAF8AbQBpAGQALAAgAG0AaQBkAHIAYQBuAGcAZQAsACAAdQBwAHAAZQByAF8AbQBpAGQALAAgAG0AYQB4AF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMALAAgAFIATwBVAE4ARAAoAHIAYQB3AF8AdgBhAGwAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsAHMALAAgAFYAUwBUAEEAQwBLACgAXAAiAE0AaQBuAFwAIgAsACAAXAAiAEwAbwB3AGUAcgAgAE0AaQBkAFwAIgAsACAAXAAiAE0AaQBkAHIAYQBuAGcAZQBcACIALAAgAFwAIgBVAHAAcABlAHIAIABNAGkAZABcACIALAAgAFwAIgBNAGEAeABcACIAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0ACwAIABJAEYAKABsAGEAYgBlAGwAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAASABTAFQAQQBDAEsAKABsAGEAYgBlAGwAcwAsACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAKQAsACAAcgBvAHUAbgBkAGUAZABfAHYAYQBsAHMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBWAE8ATABVAE0ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABiAGEAcwBpAGMAIAB2AG8AbAB1AG0AZQB0AHIAaQBjACAAcwB0AGEAdABzACAAZgBvAHIAIABhACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAHIAYQBuAGcAZQAgACAAIAA6ACAAUgBlAHEAdQBpAHIAZQBkACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQBcAG4ALQAgAGwAYQBiAGUAbAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIAB1AHMAZQAgAFwAIgBMAEIATABcACIAIABmAG8AcgAgAGwAYQBiAGUAbABlAGQAIAAyAC0AYwBvAGwAdQBtAG4AIABvAHUAdABwAHUAdABcAG4ALQAgAHAAcgBlAGMAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsADsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAA6ACAAMwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQwBvAHUAbgB0AFwAbgAtACAAUwB1AG0AXABuAC0AIABNAGUAYQBuACAAKAC8AykAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AVgBPAEwAVQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbABhAGIAZQBsAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGMAbwB1AG4AdABfAHYAYQBsACwAIABDAE8AVQBOAFQAKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcwB1AG0AXwB2AGEAbAAsACAAUwBVAE0AKAByAGEAbgBnAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbQBlAGEAbgBfAHYAYQBsACwAIABJAEYAKABjAG8AdQBuAHQAXwB2AGEAbAAgAD4AIAAwACwAIABBAFYARQBSAEEARwBFACgAcgBhAG4AZwBlACkALAAgAE4AQQAoACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAHIAYQB3AF8AdgBhAGwAcwAsACAAVgBTAFQAQQBDAEsAKABjAG8AdQBuAHQAXwB2AGEAbAAsACAAcwB1AG0AXwB2AGEAbAAsACAAbQBlAGEAbgBfAHYAYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACwAIABSAE8AVQBOAEQAKAByAGEAdwBfAHYAYQBsAHMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBDAG8AdQBuAHQAXAAiACwAIABcACIAUwB1AG0AXAAiACwAIABcACIATQBlAGEAbgAgACgAvAMpAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAIABIAFMAVABBAEMASwAoAGwAYQBiAGUAbABzACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFMASABBAFAARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABjAGUAbgB0AHIAYQBsACAAdABlAG4AZABlAG4AYwB5ACAAYQBuAGQAIABzAGgAYQBwAGUAIABkAGUAcwBjAHIAaQBwAHQAbwByAHMAIABmAG8AcgAgAGEAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAIAAgADoAIABSAGUAcQB1AGkAcgBlAGQAIABuAHUAbQBlAHIAaQBjACAAYQByAHIAYQB5AFwAbgAtACAAbABhAGIAZQBsACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAOwAgAHUAcwBlACAAXAAiAEwAQgBMAFwAIgAgAGYAbwByACAAbABhAGIAZQBsAGUAZAAgADIALQBjAG8AbAB1AG0AbgAgAG8AdQB0AHAAdQB0AFwAbgAtACAAcAByAGUAYwAgACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAOwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAKABkAGUAZgBhAHUAbAB0ADoAIAAzACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABNAGUAYQBuACAAKAC8AykAXABuAC0AIABNAGUAZABpAGEAbgBcAG4ALQAgAFMAawBlAHcALgBQAFwAbgAtACAASwB1AHIAdAAuAFAAXABuAFwAbgBOAG8AdABlADoAXABuAC0AIABSAGUAdAB1AHIAbgBzACAAIwBOAC8AQQAgAGYAbwByACAAUwBrAGUAdwAgAG8AcgAgAEsAdQByAHQAbwBzAGkAcwAgAGkAZgAgAGYAZQB3AGUAcgAgAHQAaABhAG4AIAAzACAAdgBhAGwAdQBlAHMAIABhAHIAZQAgAHAAcgBlAHMAZQBuAHQALgBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBTAEgAQQBQAEUAIAA9ACAATABBAE0AQgBEAEEAKAByAGEAbgBnAGUALAAgAFsAbABhAGIAZQBsAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAGEAYgBlAGwAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbABhAGIAZQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGMAbwB1AG4AdABfAHYAYQBsACwAIABDAE8AVQBOAFQAKAByAGEAbgBnAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgALwDLAAgAEkARgAoAGMAbwB1AG4AdABfAHYAYQBsACAAPgAgADAALAAgAEEAVgBFAFIAQQBHAEUAKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuACAAIAAgACAAIAAgACAAIABtAGUAZAAsACAASQBGACgAYwBvAHUAbgB0AF8AdgBhAGwAIAA+ACAAMAAsACAATQBFAEQASQBBAE4AKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuACAAIAAgACAAIAAgACAAIABzAGsAZQB3ACwAIABJAEYAKABjAG8AdQBuAHQAXwB2AGEAbAAgAD4AIAAyACwAIABTAEsARQBXAC4AUAAoAHIAYQBuAGcAZQApACwAIABOAEEAKAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGsAdQByAHQALAAgAEkARgAoAGMAbwB1AG4AdABfAHYAYQBsACAAPgAgADMALAAgAEsAVQBSAFQAKAByAGEAbgBnAGUAKQAsACAATgBBACgAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcAXwB2AGEAbABzACwAIABWAFMAVABBAEMASwAoALwDLAAgAG0AZQBkACwAIABzAGsAZQB3ACwAIABrAHUAcgB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwB1AG4AZABlAGQAXwB2AGEAbABzACwAIABSAE8AVQBOAEQAKAByAGEAdwBfAHYAYQBsAHMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbABzACwAIABWAFMAVABBAEMASwAoAFwAIgBNAGUAYQBuACAAKAC8AykAXAAiACwAIABcACIATQBlAGQAaQBhAG4AXAAiACwAIABcACIAUwBrAGUAdwAgACgAUAApAFwAIgAsACAAXAAiAEsAdQByAHQAbwBzAGkAcwAgACgAUAApAFwAIgApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEkARgAoAGwAYQBiAGUAbAAgAD0AIABcACIATABCAEwAXAAiACwAIABIAFMAVABBAEMASwAoAGwAYQBiAGUAbABzACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAIAByAG8AdQBuAGQAZQBkAF8AdgBhAGwAcwApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBNAEkARABSAEEATgBHAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABtAGkAZAByAGEAbgBnAGUAIABvAGYAIABhACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQA6ACAAdABoAGUAIABhAHYAZQByAGEAZwBlACAAbwBmACAAaQB0AHMAIABNAGkAbgAgAGEAbgBkACAATQBhAHgALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIABhAHIAcgBhAHkAIAA6ACAAcgBlAHEAdQBpAHIAZQBkACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQBcAG4ALQAgAHAAcgBlAGMAIAAgADoAIABvAHAAdABpAG8AbgBhAGwAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAzACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABBACAAcwBpAG4AZwBsAGUAIABuAHUAbQBlAHIAaQBjACAAdgBhAGwAdQBlADoAIAAoAE0ASQBOACAAKwAgAE0AQQBYACkAIAAvACAAMgBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBNAEkARABSAEEATgBHAEUAIAA9ACAATABBAE0AQgBEAEEAKABhAHIAcgBhAHkALAAgAFsAcAByAGUAYwBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAGMAbwB1AG4AdABfAHYAYQBsACwAIABDAE8AVQBOAFQAKABhAHIAcgBhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbQBpAGQAcgBhAG4AZwBlACwAIABJAEYAKABjAG8AdQBuAHQAXwB2AGEAbAAgAD0AIAAwACwAIABOAEEAKAApACwAIABBAFYARQBSAEEARwBFACgATQBJAE4AKABhAHIAcgBhAHkAKQAsACAATQBBAFgAKABhAHIAcgBhAHkAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAG0AaQBkAHIAYQBuAGcAZQAsACAAcAByAGUAYwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8ARgBSAEUAUQBfAFQAQQBCAEwARQBcAG4AXABuAEcAZQBuAGUAcgBhAHQAZQBzACAAYQAgAGYAcgBlAHEAdQBlAG4AYwB5ACAAdABhAGIAbABlACAAZgByAG8AbQAgAGEAIABuAHUAbQBlAHIAaQBjACAAcgBhAG4AZwBlAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAcgBhAG4AZwBlACAAOgAgAHIAZQBxAHUAaQByAGUAZAAgAG4AdQBtAGUAcgBpAGMAIABpAG4AcAB1AHQAXABuAC0AIABtAG8AZABlACAAIAA6ACAAbwBwAHQAaQBvAG4AYQBsACAAawBlAHkAdwBvAHIAZAAgACgAXAAiAEwAQgBMAFwAIgAgAHQAbwAgAGkAbgBjAGwAdQBkAGUAIABjAG8AbAB1AG0AbgAgAGgAZQBhAGQAZQByAHMAOwAgAGQAZQBmAGEAdQBsAHQAIAA9ACAAbgBvACAAaABlAGEAZABlAHIAcwApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgADMALQBjAG8AbAB1AG0AbgAgAHMAcABpAGwAbABlAGQAIABhAHIAcgBhAHkAOgBcAG4AIAAgACAAIAAiICAAQwBvAGwAdQBtAG4AIAAxADoAIABVAG4AaQBxAHUAZQAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACIgIABDAG8AbAB1AG0AbgAgADIAOgAgAEYAcgBlAHEAdQBlAG4AYwB5ACAAKABjAG8AdQBuAHQAKQBcAG4AIAAgACAAIAAiICAAQwBvAGwAdQBtAG4AIAAzADoAIABXAGUAaQBnAGgAdABlAGQAIABwAHIAbwBkAHUAYwB0ACAAKAB2AGEAbAB1AGUAIADXACAAYwBvAHUAbgB0ACkAXABuAFwAbgBOAG8AdABlAHMAOgBcAG4ALQAgAFMAbwByAHQAZQBkACAAaQBuACAAYQBzAGMAZQBuAGQAaQBuAGcAIABvAHIAZABlAHIAXABuAC0AIABJAG4AYwBsAHUAZABlAHMAIABoAGUAYQBkAGUAcgBzACAAaQBmACAAbQBvAGQAZQAgAD0AIABcACIATABCAEwAXAAiAFwAbgAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAG0AbwBkAGUAIABhAG4AYQBsAHkAcwBpAHMALAAgAHcAZQBpAGcAaAB0AGUAZAAgAG0AZQBhAG4AcwAsACAAYQBuAGQAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAG8AdgBlAHIAdgBpAGUAdwBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBGAFIARQBRAF8AVABBAEIATABFACAAPQAgAEwAQQBNAEIARABBACgAcgBhAG4AZwBlACwAIABbAG0AbwBkAGUAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABIAGEAbgBkAGwAZQAgAGwAYQBiAGUAbAAgAG0AbwBkAGUAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAFwAIgAsACAAVQBQAFAARQBSACgAbQBvAGQAZQApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABQAHIAZQBwAGEAcgBlACAAdQBuAGkAcQB1AGUAIAB2AGEAbAB1AGUAcwAgAGkAbgAgAHMAbwByAHQAZQBkACAAbwByAGQAZQByAFwAbgAgACAAIAAgACAAIAAgACAAdQBfAHYAYQBsAHMALAAgAFMATwBSAFQAKABVAE4ASQBRAFUARQAoAHIAYQBuAGcAZQApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABGAHIAZQBxAHUAZQBuAGMAeQAgAGMAbwB1AG4AdABzACAAcABlAHIAIAB1AG4AaQBxAHUAZQAgAHYAYQBsAHUAZQBcAG4AIAAgACAAIAAgACAAIAAgAHcAZQBpAGcAaAB0AHMALAAgAEIAWQBSAE8AVwAoAHUAXwB2AGEAbABzACwAIABMAEEATQBCAEQAQQAoAGEALAAgAEMATwBVAE4AVABJAEYAKAByAGEAbgBnAGUALAAgAGEAKQApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABXAGUAaQBnAGgAdABlAGQAIAB2AGEAbAB1AGUAIADXACAAZgByAGUAcQB1AGUAbgBjAHkAXABuACAAIAAgACAAIAAgACAAIABwAHIAbwBkAHUAYwB0AHMALAAgAHUAXwB2AGEAbABzACAAKgAgAHcAZQBpAGcAaAB0AHMALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABBAGQAZAAgAGMAbwBsAHUAbQBuACAAaABlAGEAZABlAHIAcwAgAGkAZgAgAFwAIgBMAEIATABcACIAIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAAdgBhAGwAdQBlAHMAXwBjAG8AbAAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIATABCAEwAXAAiACwAIABWAFMAVABBAEMASwAoAFwAIgBWAGEAbAB1AGUAXAAiACwAIAB1AF8AdgBhAGwAcwApACwAIAB1AF8AdgBhAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIAB3AGUAaQBnAGgAdABzAF8AYwBvAGwALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAAVgBTAFQAQQBDAEsAKABcACIAVwBlAGkAZwBoAHQAXAAiACwAIAB3AGUAaQBnAGgAdABzACkALAAgAHcAZQBpAGcAaAB0AHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAByAG8AZAB1AGMAdABzAF8AYwBvAGwALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAEwAQgBMAFwAIgAsACAAVgBTAFQAQQBDAEsAKABcACIAUAByAG8AZAB1AGMAdABcACIALAAgAHAAcgBvAGQAdQBjAHQAcwApACwAIABwAHIAbwBkAHUAYwB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEYAaQBuAGEAbAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKAB2AGEAbAB1AGUAcwBfAGMAbwBsACwAIAB3AGUAaQBnAGgAdABzAF8AYwBvAGwALAAgAHAAcgBvAGQAdQBjAHQAcwBfAGMAbwBsACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBXAFQARABfAEEAVgBHAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdwBlAGkAZwBoAHQAZQBkACAAYQB2AGUAcgBhAGcAZQAgAG8AZgAgAGEAIAB2AGEAbAB1AGUAIABzAGUAdAAgAGIAYQBzAGUAZAAgAG8AbgAgAGEAIABtAGEAdABjAGgAaQBuAGcAIAB3AGUAaQBnAGgAdAAgAHMAZQB0AC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAdwB0AHMAIAAgACAAIAA6ACAAYQByAHIAYQB5ACAAbwBmACAAdwBlAGkAZwBoAHQAcwBcAG4ALQAgAHYAYQBsAHUAZQBzACAAOgAgAGEAcgByAGEAeQAgAG8AZgAgAHYAYQBsAHUAZQBzACAAKABzAGEAbQBlACAAbABlAG4AZwB0AGgAIABhAHMAIAB3AGUAaQBnAGgAdABzACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABXAGUAaQBnAGgAdABlAGQAIABhAHYAZQByAGEAZwBlACAAPQAgAFMAVQBNAFAAUgBPAEQAVQBDAFQAKAB3AHQAcwAsACAAdgBhAGwAdQBlAHMAKQAgAC8AIABTAFUATQAoAHcAdABzACkAXABuAC0AIABSAGUAdAB1AHIAbgBzACAAIwBOAC8AQQAgAGkAZgAgAGkAbgBwAHUAdAAgAGwAZQBuAGcAdABoAHMAIABtAGkAcwBtAGEAdABjAGgAIABvAHIAIAB3AGUAaQBnAGgAdAAgAHMAdQBtACAAaQBzACAAegBlAHIAbwBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBXAFQARABfAEEAVgBHACAAPQAgAEwAQQBNAEIARABBACgAdwB0AHMALAAgAHYAYQBsAHUAZQBzACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGwAZQBuAF8AbQBhAHQAYwBoACwAIABDAE8AVQBOAFQAQQAoAHcAdABzACkAIAA9ACAAQwBPAFUATgBUAEEAKAB2AGEAbAB1AGUAcwApACwAXABuACAAIAAgACAAIAAgACAAIAB0AG8AdABhAGwAXwB3AHQALAAgAFMAVQBNACgAdwB0AHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAGwAZQBuAF8AbQBhAHQAYwBoACkAIAArACAAKAB0AG8AdABhAGwAXwB3AHQAIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBVAE0AUABSAE8ARABVAEMAVAAoAHcAdABzACwAIAB2AGEAbAB1AGUAcwApACAALwAgAHQAbwB0AGEAbABfAHcAdABcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBTAEUATABGAF8AVwBUAEQAXwBBAFYARwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAcwBlAGwAZgAtAHcAZQBpAGcAaAB0AGUAZAAgAGEAdgBlAHIAYQBnAGUAIABvAGYAIAB2AGEAbAB1AGUAcwAsACAAdwBoAGUAcgBlACAAZQBhAGMAaAAgAHYAYQBsAHUAZQAgAGkAcwAgAHQAcgBlAGEAdABlAGQAIABhAHMAIABpAHQAcwAgAG8AdwBuACAAdwBlAGkAZwBoAHQALgBcAG4AXABuAEEAcgBnAHUAbQBlAG4AdABzADoAXABuAC0AIAByAGEAbgBnAGUAIAA6ACAAbgB1AG0AZQByAGkAYwAgAGEAcgByAGEAeQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAKMDKAB4AGIdsgApACAALwAgAKMDKAB4AGIdKQBcAG4ALQAgAFIAZQB0AHUAcgBuAHMAIAAjAE4ALwBBACAAaQBmACAAdABvAHQAYQBsACAAcwB1AG0AIAA9ACAAMABcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBTAEUATABGAF8AVwBUAEQAXwBBAFYARwAgAD0AIABMAEEATQBCAEQAQQAoAHIAYQBuAGcAZQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABzAHUAbQBfAHYAYQBsAHMALAAgAFMAVQBNACgAcgBhAG4AZwBlACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABzAHUAbQBfAHYAYQBsAHMAIAA9ACAAMAAsACAATgBBACgAKQAsACAAUwBVAE0AUABSAE8ARABVAEMAVAAoAHIAYQBuAGcAZQAsACAAcgBhAG4AZwBlACkAIAAvACAAcwB1AG0AXwB2AGEAbABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQBzAHUAbAB0AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8AUABDAFQAXwBSAEUATQBBAFAAXABuAFwAbgBSAGUAcwBjAGEAbABlAHMAIABhACAAdgBhAGwAdQBlACAAZgByAG8AbQAgAG8AbgBlACAAbgB1AG0AZQByAGkAYwAgAHIAYQBuAGcAZQAgAGkAbgB0AG8AIABhAG4AbwB0AGgAZQByACwAIABwAHIAZQBzAGUAcgB2AGkAbgBnACAAaQB0AHMAXABuAHIAZQBsAGEAdABpAHYAZQAgAHAAbwBzAGkAdABpAG8AbgAgACgAcABlAHIAYwBlAG4AdABpAGwAZQApACAAYgBlAHQAdwBlAGUAbgAgAHQAaABlACAAdAB3AG8AIABpAG4AdABlAHIAdgBhAGwAcwAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAFMAdABhAHIAdABNAGkAbgAsACAAUwB0AGEAcgB0AE0AYQB4ACAAOgAgAG8AcgBpAGcAaQBuAGEAbAAgAG4AdQBtAGUAcgBpAGMAIAByAGEAbgBnAGUAXABuAC0AIABUAGEAcgBnAGUAdAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADoAIAB2AGEAbAB1AGUAIAB3AGkAdABoAGkAbgAgAHQAaABlACAAbwByAGkAZwBpAG4AYQBsACAAcgBhAG4AZwBlAFwAbgAtACAARQBuAGQATQBpAG4ALAAgAEUAbgBkAE0AYQB4ACAAIAAgACAAIAA6ACAAZABlAHMAdABpAG4AYQB0AGkAbwBuACAAcgBhAG4AZwBlAFwAbgAtACAAZABlAGMAcAByAGUAYwAgACgAbwBwAHQAaQBvAG4AYQBsACkAIAA6ACAAZABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADEANQApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAVABoAGUAIABwAGUAcgBjAGUAbgB0AGkAbABlAC0AZQBxAHUAaQB2AGEAbABlAG4AdAAgAHYAYQBsAHUAZQAgAGkAbgAgAHQAaABlACAAcwBlAGMAbwBuAGQAIAByAGEAbgBnAGUAXABuAFwAbgBFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAUwBUAEEAVABfAFAAQwBUAF8AUgBFAE0AQQBQACgAMwAsACAAMQAxACwAIAA1ACwAIAAyACwAIAAxADkAKQBcAG4AIAAgACAAIACSISAANgAuADIANQAgACgAcwBpAG4AYwBlACAANQAgAGkAcwAgADIANQAlACAAYgBlAHQAdwBlAGUAbgAgADMAEyAxADEALAAgAGEAbgBkACAANgAuADIANQAgAGkAcwAgADIANQAlACAAYgBlAHQAdwBlAGUAbgAgADIAEyAxADkAKQBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBQAEMAVABfAFIARQBNAEEAUAAgAD0AIABMAEEATQBCAEQAQQAoAFMAdABhAHIAdABNAGkAbgAsACAAUwB0AGEAcgB0AE0AYQB4ACwAIABUAGEAcgBnAGUAdAAsACAARQBuAGQATQBpAG4ALAAgAEUAbgBkAE0AYQB4ACwAIABbAGQAZQBjAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkAGUAYwBwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGQAZQBjAHAAcgBlAGMAKQAsACAAMQA1ACwAIABkAGUAYwBwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAHAAYwB0ACwAIAAoAFQAYQByAGcAZQB0ACAALQAgAFMAdABhAHIAdABNAGkAbgApACAALwAgACgAUwB0AGEAcgB0AE0AYQB4ACAALQAgAFMAdABhAHIAdABNAGkAbgApACwAXABuACAAIAAgACAAIAAgACAAIABjAGEAbABjACwAIABwAGMAdAAgACoAIAAoAEUAbgBkAE0AYQB4ACAALQAgAEUAbgBkAE0AaQBuACkAIAArACAARQBuAGQATQBpAG4ALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAGMAYQBsAGMALAAgAGQAZQBjAHAAcgBlAGMAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFAAQwBUAF8ATwBGAF8AUgBBAE4ARwBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAcABlAHIAYwBlAG4AdABpAGwAZQAgACgAYQBzACAAYQAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AKQAgAHQAaABhAHQAIABhACAAdgBhAGwAdQBlACAAcgBlAHAAcgBlAHMAZQBuAHQAcwBcAG4AdwBpAHQAaABpAG4AIABhACAAcwBwAGUAYwBpAGYAaQBlAGQAIABuAHUAbQBlAHIAaQBjACAAcgBhAG4AZwBlAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAbQBpAG4AIAAgACAAIAAgACAAOgAgAGwAbwB3AGUAcgAgAGIAbwB1AG4AZAAgAG8AZgAgAHIAYQBuAGcAZQBcAG4ALQAgAG0AYQB4ACAAIAAgACAAIAAgADoAIAB1AHAAcABlAHIAIABiAG8AdQBuAGQAIABvAGYAIAByAGEAbgBnAGUAXABuAC0AIAB2AGEAbAB1AGUAIAAgACAAIAA6ACAAdgBhAGwAdQBlACAAdABvACAAZQB2AGEAbAB1AGEAdABlAFwAbgAtACAAZABlAGMAcAByAGUAYwAgACAAOgAgAG8AcAB0AGkAbwBuAGEAbAAgAGQAZQBjAGkAbQBhAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAxADUAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAFQAaABlACAAcAByAG8AcABvAHIAdABpAG8AbgBhAGwAIABwAG8AcwBpAHQAaQBvAG4AIABvAGYAIABgAHYAYQBsAHUAZQBgACAAaQBuACAAdABoAGUAIAByAGEAbgBnAGUAIABbAG0AaQBuACwAIABtAGEAeABdAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIAAgAFMAVABBAFQAXwBQAEMAVABfAE8ARgBfAFIAQQBOAEcARQAoADMALAAgADEAMgAsACAANwApAFwAbgAgACAAIAAgAJIhIAAwAC4ANAA0ADQALgAuAC4AIAAoAGIAZQBjAGEAdQBzAGUAIAA3ACAAaQBzACAANAA0AC4ANAAlACAAbwBmACAAdABoAGUAIAB3AGEAeQAgAGYAcgBvAG0AIAAzACAAdABvACAAMQAyACkAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AUABDAFQAXwBPAEYAXwBSAEEATgBHAEUAIAA9ACAATABBAE0AQgBEAEEAKABtAGkAbgAsACAAbQBhAHgALAAgAHYAYQBsAHUAZQAsACAAWwBkAGUAYwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGMAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBwAHIAZQBjACkALAAgADEANQAsACAAZABlAGMAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABjAGEAbABjACwAIAAoAHYAYQBsAHUAZQAgAC0AIABtAGkAbgApACAALwAgACgAbQBhAHgAIAAtACAAbQBpAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAYwBhAGwAYwAsACAAZABlAGMAcAByAGUAYwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8AVgBBAEwAVQBFAF8ATwBGAF8AUABDAFQAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB2AGEAbAB1AGUAIAB0AGgAYQB0ACAAYwBvAHIAcgBlAHMAcABvAG4AZABzACAAdABvACAAYQAgAGcAaQB2AGUAbgAgAHAAZQByAGMAZQBuAHQAYQBnAGUAIAAoAGEAcwAgAGEAIABkAGUAYwBpAG0AYQBsACkAIABcAG4AdwBpAHQAaABpAG4AIABhACAAcwBwAGUAYwBpAGYAaQBlAGQAIABuAHUAbQBlAHIAaQBjACAAcgBhAG4AZwBlAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAbQBpAG4AIAAgACAAIAAgACAAOgAgAGwAbwB3AGUAcgAgAGIAbwB1AG4AZAAgAG8AZgAgAHIAYQBuAGcAZQBcAG4ALQAgAG0AYQB4ACAAIAAgACAAIAAgADoAIAB1AHAAcABlAHIAIABiAG8AdQBuAGQAIABvAGYAIAByAGEAbgBnAGUAXABuAC0AIABwAGMAdAAgACAAIAAgACAAIAA6ACAAcABlAHIAYwBlAG4AdABhAGcAZQAgAGUAeABwAHIAZQBzAHMAZQBkACAAYQBzACAAYQAgAGQAZQBjAGkAbQBhAGwAIAAoAGUALgBnAC4AIAAwAC4ANAAwADYANQAgAGYAbwByACAANAAwAC4ANgA1ACUAKQBcAG4ALQAgAGQAZQBjAHAAcgBlAGMAIAAgADoAIABvAHAAdABpAG8AbgBhAGwAIABkAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMQA1ACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABUAGgAZQAgAHYAYQBsAHUAZQAgAGEAdAAgAHQAaABlACAAZwBpAHYAZQBuACAAcABlAHIAYwBlAG4AdABpAGwAZQAgAGIAZQB0AHcAZQBlAG4AIABtAGkAbgAgAGEAbgBkACAAbQBhAHgAXABuAFwAbgBFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAUwBUAEEAVABfAFYAQQBMAFUARQBfAE8ARgBfAFAAQwBUACgAMwAsACAAMQAyACwAIAAwAC4ANAAwADYANQApAFwAbgAgACAAIAAgAJIhIAA2AC4ANgA1ADgANQAgACgAdwBoAGkAYwBoACAAaQBzACAANAAwAC4ANgA1ACUAIABiAGUAdAB3AGUAZQBuACAAMwAgAGEAbgBkACAAMQAyACkAXABuAFwAbgAqAC8AXABuAFwAbgBTAFQAQQBUAF8AVgBBAEwAVQBFAF8ATwBGAF8AUABDAFQAIAA9ACAATABBAE0AQgBEAEEAKABtAGkAbgAsACAAbQBhAHgALAAgAHAAYwB0ACwAIABbAGQAZQBjAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkAGUAYwBwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGQAZQBjAHAAcgBlAGMAKQAsACAAMQA1ACwAIABkAGUAYwBwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAGMAYQBsAGMALAAgAHAAYwB0ACAAKgAgACgAbQBhAHgAIAAtACAAbQBpAG4AKQAgACsAIABtAGkAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAYwBhAGwAYwAsACAAZABlAGMAcAByAGUAYwApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABTAFQAQQBUAF8AQgBFAE4ARgBPAFIARABfAFQAQQBCAEwARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaABlAG8AcgBlAHQAaQBjAGEAbAAgAEIAZQBuAGYAbwByAGQAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAHAAcgBvAGIAYQBiAGkAbABpAHQAaQBlAHMAIABmAG8AcgAgAGwAZQBhAGQAaQBuAGcAIABkAGkAZwBpAHQAcwAgADEAIAB0AGgAcgBvAHUAZwBoACAAOQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAG0AbwBkAGUAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABcAG4AIAAgACAAIAAtACAAXAAiAEwAQgBMAFwAIgAgAJIhIAByAGUAdAB1AHIAbgBzACAAYQAgADIALQBjAG8AbAB1AG0AbgAgAGEAcgByAGEAeQA6ACAARABpAGcAaQB0ACAAfAAgAFAAcgBvAGIAYQBiAGkAbABpAHQAeQBcAG4AIAAgACAAIAAtACAAYgBsAGEAbgBrAC8AbwBtAGkAdAB0AGUAZAAgAJIhIAByAGUAdAB1AHIAbgBzACAAcgBhAHcAIABwAHIAbwBiAGEAYgBpAGwAaQB0AGkAZQBzACAAbwBuAGwAeQAgACgAMQAtAGMAbwBsAHUAbQBuACkAXABuAFwAbgBSAGUAdAB1AHIAbgBzADoAXABuAC0AIABBACAAdgBlAHIAdABpAGMAYQBsACAAbABpAHMAdAAgAG8AZgAgADkAIABCAGUAbgBmAG8AcgBkACAAcAByAG8AYgBhAGIAaQBsAGkAdABpAGUAcwAgACgAbABvAGcALQBiAGEAcwBlAGQAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgApAFwAbgAtACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAGwAYQBiAGUAbABlAGQAIAB3AGkAdABoACAAZABpAGcAaQB0AHMAIAAxACAAdABoAHIAbwB1AGcAaAAgADkAXABuAFwAbgBGAG8AcgBtAHUAbABhADoAXABuAC0AIABQACgAZAApACAAPQAgAEwATwBHADEAMAAoADEAIAArACAAMQAvAGQAKQAsACAAZgBvAHIAIABkACAAaQBuACAAewAxACwAIAAyACwAIAAuAC4ALgAsACAAOQB9AFwAbgBcAG4AQwBvAG0AbQBvAG4AbAB5ACAAdQBzAGUAZAAgAGYAbwByADoAXABuAC0AIABEAGUAdABlAGMAdABpAG4AZwAgAHUAbgBuAGEAdAB1AHIAYQBsACAAcABhAHQAdABlAHIAbgBzACAAaQBuACAAZABhAHQAYQBzAGUAdABzAFwAbgAtACAARgByAGEAdQBkACAAZABlAHQAZQBjAHQAaQBvAG4AIABhAG4AZAAgAGYAbwByAGUAbgBzAGkAYwAgAGEAYwBjAG8AdQBuAHQAaQBuAGcAXABuAC0AIABNAG8AZABlAGwAaQBuAGcAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgBzACAAbwBmACAAbgBhAHQAdQByAGEAbABsAHkAIABvAGMAYwB1AHIAcgBpAG4AZwAgAG4AdQBtAGUAcgBpAGMAYQBsACAAZABhAHQAYQBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBCAEUATgBGAE8AUgBEAF8AVABBAEIATABFACAAPQAgAEwAQQBNAEIARABBACgAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABtAG8AZABlACkALAAgAFwAIgBcACIALAAgAFUAUABQAEUAUgAoAG0AbwBkAGUAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARABpAGcAaQB0AHMAIAAxACAAdABoAHIAbwB1AGcAaAAgADkAXABuACAAIAAgACAAIAAgACAAIABkAGkAZwBpAHQAcwAsACAAUwBFAFEAVQBFAE4AQwBFACgAOQAsACAALAAgADEALAAgADEAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEIAZQBuAGYAbwByAGQAIABwAHIAbwBiAGEAYgBpAGwAaQB0AGkAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAcAByAG8AYgBzACwAIABCAFkAUgBPAFcAKABkAGkAZwBpAHQAcwAsACAATABBAE0AQgBEAEEAKABkACwAIABMAE8ARwAxADAAKAAxACAAKwAgACgAMQAgAC8AIABkACkAKQApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAIABsAGEAYgBlAGwAZQBkACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUAIAA9ACAAXAAiAEwAQgBMAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAGQAaQBnAGkAdABzACwAIABwAHIAbwBiAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABwAHIAbwBiAHMAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUwBUAEEAVABfAFIATgBEAF8AQgBFAE4ARgBPAFIARABcAG4AXABuAEcAZQBuAGUAcgBhAHQAZQBzACAAbwBuAGUAIABvAHIAIABtAG8AcgBlACAAcgBhAG4AZABvAG0AIABkAGkAZwBpAHQAcwAgAGIAYQBzAGUAZAAgAG8AbgAgAHQAaABlACAAQgBlAG4AZgBvAHIAZAAgAGQAaQBzAHQAcgBpAGIAdQB0AGkAbwBuAC4AXABuAFwAbgBBAHIAZwB1AG0AZQBuAHQAcwA6AFwAbgAtACAAZABpAGcAaQB0AHMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAaQBnAGkAdABzACAAdABvACAAcgBlAHQAdQByAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMQApAFwAbgBcAG4AUgBlAHQAdQByAG4AcwA6AFwAbgAtACAAQQAgAHMAaQBuAGcAbABlAC0AZABpAGcAaQB0ACAAbgB1AG0AYgBlAHIAIABpAGYAIABkAGkAZwBpAHQAcwAgAD0AIAAxAFwAbgAtACAAQQAgAG0AdQBsAHQAaQAtAGQAaQBnAGkAdAAgAG4AdQBtAGIAZQByACAAYwBvAG0AcABvAHMAZQBkACAAbwBmACAAQgBlAG4AZgBvAHIAZAAtAGQAaQBzAHQAcgBpAGIAdQB0AGUAZAAgAGQAaQBnAGkAdABzACAAbwB0AGgAZQByAHcAaQBzAGUAXABuAFwAbgBEAGkAcwB0AHIAaQBiAHUAdABpAG8AbgA6AFwAbgAtACAAQgBhAHMAZQBkACAAbwBuACAAbABlAGEAZABpAG4AZwAgAGQAaQBnAGkAdAAgAHAAcgBvAGIAYQBiAGkAbABpAHQAaQBlAHMAOgBcAG4AIAAgACAAIABQACgAZAApACAAPQAgAEwATwBHADEAMAAoADEAIAArACAAMQAvAGQAKQAgAGYAbwByACAAZAAgAAgiIAB7ADEALgAuADkAfQBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBSAE4ARABfAEIARQBOAEYATwBSAEQAIAA9ACAATABBAE0AQgBEAEEAKABbAGQAaQBnAGkAdABzAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABpAGcAaQB0AHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAZABpAGcAaQB0AHMAKQAsACAAMQAsACAAZABpAGcAaQB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEQAaQBnAGkAdAAgAHIAYQBuAGcAZQAgADEAEyA5AFwAbgAgACAAIAAgACAAIAAgACAAbgB1AG0AbABpAHMAdAAsACAAUwBFAFEAVQBFAE4AQwBFACgAOQAsACAALAAgADEALAAgADEAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAdQBtAHUAbABhAHQAaQB2AGUAIABCAGUAbgBmAG8AcgBkACAAcAByAG8AYgBhAGIAaQBsAGkAdABpAGUAcwBcAG4AIAAgACAAIAAgACAAIAAgAHAAcgBvAGIAbABpAHMAdAAsACAAewAwAC4AMwAwADEALAAgADAALgA0ADcANwAsACAAMAAuADYAMAAyACwAIAAwAC4ANgA5ADkALAAgADAALgA3ADcAOAAsACAAMAAuADgANAA1ACwAIAAwAC4AOQAwADMALAAgADAALgA5ADUANAAsACAAMQB9ACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARwBlAG4AZQByAGEAdABlACAAcgBhAG4AZABvAG0AIABhAHIAcgBhAHkAIABvAGYAIABwAGUAcgBjAGUAbgB0AGkAbABlAHMAXABuACAAIAAgACAAIAAgACAAIAByAGEAbgBkAF8AbgB1AG0AcwAsACAAUgBBAE4ARABBAFIAUgBBAFkAKABkAGkAZwBpAHQAcwAsACAAMQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAATQBhAHQAYwBoACAAdABvACAAZABpAGcAaQB0ACAAdgBpAGEAIABwAGUAcgBjAGUAbgB0AGkAbABlACAAbQBhAHAAcABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgAGkAbgBkAGkAYwBlAHMALAAgAE0AQQBUAEMASAAoAFgATABPAE8ASwBVAFAAKAByAGEAbgBkAF8AbgB1AG0AcwAsACAAcAByAG8AYgBsAGkAcwB0ACwAIABwAHIAbwBiAGwAaQBzAHQALAAgACwAIAAxACkALAAgAHAAcgBvAGIAbABpAHMAdAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIABkAGkAZwBpAHQAcwBfAGcAZQBuAGUAcgBhAHQAZQBkACwAIABJAE4ARABFAFgAKABuAHUAbQBsAGkAcwB0ACwAIABpAG4AZABpAGMAZQBzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHUAdABwAHUAdAAgAGEAcwAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGQAaQBnAGkAdABzACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgAZABpAGcAaQB0AHMAXwBnAGUAbgBlAHIAYQB0AGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFQARQBYAFQASgBPAEkATgAoAFwAIgBcACIALAAgAFQAUgBVAEUALAAgAGQAaQBnAGkAdABzAF8AZwBlAG4AZQByAGEAdABlAGQAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFMAVABBAFQAXwBWAEEATABfAEIAUgBBAEMASwBFAFQAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB2AGEAbAB1AGUAcwAgAGkAbgAgAGEAIABkAGEAdABhAHMAZQB0ACAAdABoAGEAdAAgAGIAcgBhAGMAawBlAHQAIABhACAAcwBwAGUAYwBpAGYAaQBlAGQAIAB0AGEAcgBnAGUAdAAgAHYAYQBsAHUAZQAuAFwAbgBcAG4AQQByAGcAdQBtAGUAbgB0AHMAOgBcAG4ALQAgAFQAZQBzAHQAQQByAHIAYQB5ACAAOgAgAGEAcgByAGEAeQAgAG8AZgAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAcwBcAG4ALQAgAFQAYQByAGcAZQB0ACAAIAAgACAAOgAgAHQAaABlACAAdgBhAGwAdQBlACAAdABvACAAZgBpAG4AZAAgAGIAcgBhAGMAawBlAHQAaQBuAGcAIABiAG8AdQBuAGQAcwAgAGYAbwByAFwAbgAtACAAaQBuAGMAbAAgACAAIAAgACAAIAA6ACAAbwBwAHQAaQBvAG4AYQBsACwAIABcACIASQBOAEMAXAAiACAAKABkAGUAZgBhAHUAbAB0ACkAIABpAG4AYwBsAHUAZABlAHMAIAB0AGEAcgBnAGUAdAAgAGkAbgAgAHIAZQBzAHUAbAB0ACwAIABcACIARQBYAEMAXAAiACAAZQB4AGMAbAB1AGQAZQBzACAAaQB0AFwAbgAtACAAbQBvAGQAZQAgACAAIAAgACAAIAA6ACAAbwBwAHQAaQBvAG4AYQBsACAAbABhAHkAbwB1AHQAOgBcAG4AIAAgACAAIABcACIAVgBFAFIAXAAiACAAPQAgAHYAZQByAHQAaQBjAGEAbAAgAGEAcgByAGEAeQAgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgAFwAIgBIAE8AUgBcACIAIAA9ACAAaABvAHIAaQB6AG8AbgB0AGEAbAAgAGEAcgByAGEAeQBcAG4AIAAgACAAIABcACIAUwBUAFIAXAAiACAAPQAgAHMAdAByAGkAbgBnACAAZgBvAHIAbQBhAHQAIABcACIAKABsAG8AdwBlAHIAIAA6ACAAWwB0AGEAcgBnAGUAdABdACAAOgAgAHUAcABwAGUAcgApAFwAIgBcAG4ALQAgAGwAYgBsACAAIAAgACAAIAAgACAAOgAgAG8AcAB0AGkAbwBuAGEAbAAgAGsAZQB5AHcAbwByAGQAIABcACIATABCAEwAXAAiACAAdABvACAAaQBuAGMAbAB1AGQAZQAgAGwAYQBiAGUAbABzACAAaQBuACAAbwB1AHQAcAB1AHQAIAAoAGkAZwBuAG8AcgBlAGQAIABpAG4AIABcACIAUwBUAFIAXAAiACAAbQBvAGQAZQApAFwAbgAtACAAcAByAGUAYwAgACAAIAAgACAAIAA6ACAAbwBwAHQAaQBvAG4AYQBsACAAZABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAdABvACAAcgBvAHUAbgBkACAAdABvACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADMAKQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAOgBcAG4ALQAgAFQAaABlACAAdgBhAGwAdQBlAHMAIABpAG0AbQBlAGQAaQBhAHQAZQBsAHkAIABhAGIAbwB2AGUAIABhAG4AZAAgAGIAZQBsAG8AdwAgAHQAaABlACAAdABhAHIAZwBlAHQAIAAoAG8AcgAgAGEAbABzAG8AIAB0AGgAZQAgAHQAYQByAGcAZQB0ACwAIABpAGYAIABcACIASQBOAEMAXAAiACkAXABuAC0AIABPAHUAdABwAHUAdAAgAGEAcwAgAGEAcgByAGEAeQAgACgAdgBlAHIAdABpAGMAYQBsACAAbwByACAAaABvAHIAaQB6AG8AbgB0AGEAbAApACwAIABzAHQAcgBpAG4AZwAsACAAbwByACAAbABhAGIAZQBsAGUAZAAgAGEAcgByAGEAeQBcAG4AXABuACoALwBcAG4AXABuAFMAVABBAFQAXwBWAEEATABfAEIAUgBBAEMASwBFAFQAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAcwB0AEEAcgByAGEAeQAsACAAVABhAHIAZwBlAHQALAAgAFsAaQBuAGMAbABdACwAIABbAG0AbwBkAGUAXQAsACAAWwBsAGIAbABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAAMwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABVAFAAUABFAFIAKABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAFYARQBSAFwAIgAsACAAbQBvAGQAZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYgBsACwAIABVAFAAUABFAFIAKABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGwAYgBsACkALAAgAFwAIgBcACIALAAgAGwAYgBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAbABiAGwAXwB2AGEAbAAsACAAbABiAGwAIAA9ACAAXAAiAEwAQgBMAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAaQBuAGMAbAAsACAAVQBQAFAARQBSACgASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABpAG4AYwBsACkALAAgAFwAIgBJAE4AQwBcACIALAAgAGkAbgBjAGwAKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAQwBvAG0AcAB1AHQAZQAgAGIAbwB1AG4AZABpAG4AZwAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAbABvAHcAZQByACwAIABNAEEAWAAoAEYASQBMAFQARQBSACgAVABlAHMAdABBAHIAcgBhAHkALAAgAFQAZQBzAHQAQQByAHIAYQB5ACAAPAAgAFQAYQByAGcAZQB0ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAdQBwAHAAZQByACwAIABNAEkATgAoAEYASQBMAFQARQBSACgAVABlAHMAdABBAHIAcgBhAHkALAAgAFQAZQBzAHQAQQByAHIAYQB5ACAAPgAgAFQAYQByAGcAZQB0ACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEIAdQBpAGwAZAAgAHYAYQBsAHUAZQAgAGwAaQBzAHQAIABiAGEAcwBlAGQAIABvAG4AIABpAG4AYwBsAHUAcwBpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAHYAYQBsAF8AYQByAHIAYQB5ACwAIABJAEYAKABpAG4AYwBsACAAPQAgAFwAIgBJAE4AQwBcACIALAAgAFYAUwBUAEEAQwBLACgAbABvAHcAZQByACwAIABUAGEAcgBnAGUAdAAsACAAdQBwAHAAZQByACkALAAgAFYAUwBUAEEAQwBLACgAbABvAHcAZQByACwAIAB1AHAAcABlAHIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAB2AGEAbABfAGEAcgByAGEAeQBfAHIALAAgAFIATwBVAE4ARAAoAHYAYQBsAF8AYQByAHIAYQB5ACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AcgByAGUAcwBwAG8AbgBkAGkAbgBnACAAbABhAGIAZQBsACAAbABpAHMAdABcAG4AIAAgACAAIAAgACAAIAAgAGwAYgBsAF8AYQByAHIAYQB5ACwAIABJAEYAKABpAG4AYwBsACAAPQAgAFwAIgBJAE4AQwBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcACIATABvAHcAZQByAFwAIgA7ACAAXAAiAFQAYQByAGcAZQB0AFwAIgA7ACAAXAAiAFUAcABwAGUAcgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AFwAIgBMAG8AdwBlAHIAXAAiADsAIABcACIAVQBwAHAAZQByAFwAIgB9AFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAE8AdQB0AHAAdQB0ACAAcwBlAGwAZQBjAHQAbwByAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAFMAVwBJAFQAQwBIACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFMAVABSAFwAIgAsACAAXAAiACgAXAAiACAAJgAgAFQARQBYAFQASgBPAEkATgAoAFwAIgAgADoAIABcACIALAAgACwAIABGAEkAWABFAEQAKAB2AGEAbABfAGEAcgByAGEAeQBfAHIALAAgAHAAcgBlAGMAKQApACAAJgAgAFwAIgApAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIASABPAFIAXAAiACwAIABJAEYAKABsAGIAbABfAHYAYQBsACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABUAFIAQQBOAFMAUABPAFMARQAoAGwAYgBsAF8AYQByAHIAYQB5ACkALAAgAFQAUgBBAE4AUwBQAE8AUwBFACgAdgBhAGwAXwBhAHIAcgBhAHkAXwByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBBAE4AUwBQAE8AUwBFACgAdgBhAGwAXwBhAHIAcgBhAHkAXwByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFYARQBSAFwAIgAsACAASQBGACgAbABiAGwAXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAbABiAGwAXwBhAHIAcgBhAHkALAAgAHYAYQBsAF8AYQByAHIAYQB5AF8AcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdgBhAGwAXwBhAHIAcgBhAHkAXwByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHYAYQBsAF8AYQByAHIAYQB5AF8AcgAgACAALwAvACAAZgBhAGwAbABiAGEAYwBrACAAZABlAGYAYQB1AGwAdABcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuACIAfQBdACwAIgBwAHIAbwBqAGUAYwB0AE4AYQBtAGUAcwAiADoAWwAiAFMAVABBAFQAXwBRAE4AVABJAEwARQBTACIALAAiAFMAVABBAFQAXwBTAFQARABFAFIAUgAiACwAIgBTAFQAQQBUAF8ATQBJAE4ATQBBAFgAIgAsACIAUwBUAEEAVABfAFMAVQBNAE0AQQBSAFkAIgAsACIAUwBUAEEAVABfAEcARQBPADUAIgAsACIAUwBUAEEAVABfAFYATwBMAFUATQBFACIALAAiAFMAVABBAFQAXwBTAEgAQQBQAEUAIgAsACIAUwBUAEEAVABfAE0ASQBEAFIAQQBOAEcARQAiACwAIgBTAFQAQQBUAF8ARgBSAEUAUQBfAFQAQQBCAEwARQAiACwAIgBTAFQAQQBUAF8AVwBUAEQAXwBBAFYARwAiACwAIgBTAFQAQQBUAF8AUwBFAEwARgBfAFcAVABEAF8AQQBWAEcAIgAsACIAUwBUAEEAVABfAFAAQwBUAF8AUgBFAE0AQQBQACIALAAiAFMAVABBAFQAXwBQAEMAVABfAE8ARgBfAFIAQQBOAEcARQAiACwAIgBTAFQAQQBUAF8AVgBBAEwAVQBFAF8ATwBGAF8AUABDAFQAIgAsACIAUwBUAEEAVABfAEIARQBOAEYATwBSAEQAXwBUAEEAQgBMAEUAIgAsACIAUwBUAEEAVABfAFIATgBEAF8AQgBFAE4ARgBPAFIARAAiACwAIgBTAFQAQQBUAF8AVgBBAEwAXwBCAFIAQQBDAEsARQBUACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIAWQBNAEQAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>